<commit_message>
Updated reg_labourSupplyUtility.xlsx and adjusted the code accordingly
</commit_message>
<xml_diff>
--- a/input/PL/reg_education.xlsx
+++ b/input/PL/reg_education.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pineapple/IdeaProjects/SimPathsEU_testEdu/input/PL/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FA8888C-A5AF-3B47-8BB0-C7AE4CEC9B38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50D97F4A-38F2-4C44-883A-8B3E32BFBDA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="28300" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="21100" yWindow="500" windowWidth="30100" windowHeight="28300" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,20 @@
     <sheet name="E1b" sheetId="4" r:id="rId4"/>
     <sheet name="E2a" sheetId="6" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -881,7 +894,7 @@
   <dimension ref="A1:U19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="B1" sqref="B1:T19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2019,7 +2032,7 @@
         <v>-87.046836493611409</v>
       </c>
       <c r="E19">
-        <v>2.4310399428561311</v>
+        <v>2.4310399428561298</v>
       </c>
       <c r="F19">
         <v>-2.479003590669663</v>
@@ -2076,7 +2089,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:T18"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:S18"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -3154,8 +3169,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:W22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:W22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:W22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Applied new ExcelAssistant.loadCoefficientMap() -updated JAS-mine-core to version 4.3.24 -removed calling valueColumns in the loadCoefficientMap() -updated some of the excel files to remove blank cells  as they were causing the following error: Cannot invoke "java. lang.Number doubleValue()" because "mapValuesRow[java. lang. Integer.intValue()]" is null -clean up of the Parameters.java
</commit_message>
<xml_diff>
--- a/input/PL/reg_education.xlsx
+++ b/input/PL/reg_education.xlsx
@@ -1,31 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10110"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://essexuniversity-my.sharepoint.com/personal/mv25449_essex_ac_uk/Documents/WorkCEMPA/SimPathsEU/PL_regression_estimates/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pineapple/IdeaProjects/SimPathsEU_JAN/input/PL/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="11_BBDD9C3A68078AAA74C7807FC4B4BE5D21DC90B9" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DD0755B8-FC02-F74C-BF01-333F9E1E78F5}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{609C2B59-A07F-004F-9288-B8C1C52ED7C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="28300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="28300" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
     <sheet name="Gof" sheetId="2" r:id="rId2"/>
-    <sheet name="E1a" sheetId="3" r:id="rId3"/>
-    <sheet name="E1b" sheetId="4" r:id="rId4"/>
-    <sheet name="E2a_raw" sheetId="5" r:id="rId5"/>
-    <sheet name="E2a" sheetId="6" r:id="rId6"/>
+    <sheet name="E1a_old" sheetId="3" r:id="rId3"/>
+    <sheet name="E1a" sheetId="7" r:id="rId4"/>
+    <sheet name="E1b_old" sheetId="4" r:id="rId5"/>
+    <sheet name="E1b" sheetId="8" r:id="rId6"/>
+    <sheet name="E2a_raw" sheetId="5" r:id="rId7"/>
+    <sheet name="E2a_old" sheetId="6" r:id="rId8"/>
+    <sheet name="E2a" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="82">
   <si>
     <t>Description:</t>
   </si>
@@ -2211,7 +2214,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="160">
+  <cellXfs count="162">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -2372,6 +2375,8 @@
     <xf numFmtId="2" fontId="158" fillId="0" borderId="157" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="159" fillId="0" borderId="158" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="158" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="158" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2882,8 +2887,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:U19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="T19" sqref="A1:T19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4075,10 +4080,1205 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A9E8FC0-3E90-5241-8A43-799FDEC839E2}">
+  <dimension ref="A1:T19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:T19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A1" s="160" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="160" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="160" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="160" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="160" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" s="160" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" s="160" t="s">
+        <v>50</v>
+      </c>
+      <c r="H1" s="160" t="s">
+        <v>20</v>
+      </c>
+      <c r="I1" s="160" t="s">
+        <v>21</v>
+      </c>
+      <c r="J1" s="160" t="s">
+        <v>22</v>
+      </c>
+      <c r="K1" s="160" t="s">
+        <v>23</v>
+      </c>
+      <c r="L1" s="160" t="s">
+        <v>24</v>
+      </c>
+      <c r="M1" s="160" t="s">
+        <v>25</v>
+      </c>
+      <c r="N1" s="160" t="s">
+        <v>26</v>
+      </c>
+      <c r="O1" s="160" t="s">
+        <v>27</v>
+      </c>
+      <c r="P1" s="160" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q1" s="160" t="s">
+        <v>29</v>
+      </c>
+      <c r="R1" s="160" t="s">
+        <v>30</v>
+      </c>
+      <c r="S1" s="160" t="s">
+        <v>31</v>
+      </c>
+      <c r="T1" s="160" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A2" s="160" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="160">
+        <v>-0.1603360747524277</v>
+      </c>
+      <c r="C2" s="160">
+        <v>1.4286289289300892E-3</v>
+      </c>
+      <c r="D2" s="160">
+        <v>6.5153256662823233E-3</v>
+      </c>
+      <c r="E2" s="160">
+        <v>-1.7935173747858028E-4</v>
+      </c>
+      <c r="F2" s="160">
+        <v>1.7502779710062803E-4</v>
+      </c>
+      <c r="G2" s="160">
+        <v>6.1253561870731248E-5</v>
+      </c>
+      <c r="H2" s="160">
+        <v>2.5886840098702005E-5</v>
+      </c>
+      <c r="I2" s="160">
+        <v>1.7962333265363886E-4</v>
+      </c>
+      <c r="J2" s="160">
+        <v>5.3124240932293852E-5</v>
+      </c>
+      <c r="K2" s="160">
+        <v>4.5712785431306635E-4</v>
+      </c>
+      <c r="L2" s="160">
+        <v>-1.6298682901668814E-4</v>
+      </c>
+      <c r="M2" s="160">
+        <v>-1.5639961434307749E-4</v>
+      </c>
+      <c r="N2" s="160">
+        <v>-1.8268489467859056E-4</v>
+      </c>
+      <c r="O2" s="160">
+        <v>-1.9876794228678666E-4</v>
+      </c>
+      <c r="P2" s="160">
+        <v>-2.5926383840036912E-6</v>
+      </c>
+      <c r="Q2" s="160">
+        <v>-6.3352423641038942E-5</v>
+      </c>
+      <c r="R2" s="160">
+        <v>-2.1740147754592543E-5</v>
+      </c>
+      <c r="S2" s="160">
+        <v>2.0931814563870769E-4</v>
+      </c>
+      <c r="T2" s="160">
+        <v>-5.9911043825341848E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A3" s="160" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="160">
+        <v>14.808142749582386</v>
+      </c>
+      <c r="C3" s="160">
+        <v>6.5153256662823233E-3</v>
+      </c>
+      <c r="D3" s="160">
+        <v>9.7357429951287031</v>
+      </c>
+      <c r="E3" s="160">
+        <v>-0.27191717216847522</v>
+      </c>
+      <c r="F3" s="160">
+        <v>0.27734999427854845</v>
+      </c>
+      <c r="G3" s="160">
+        <v>9.8265176728999926E-3</v>
+      </c>
+      <c r="H3" s="160">
+        <v>1.1317111183015705E-3</v>
+      </c>
+      <c r="I3" s="160">
+        <v>2.1680501905967375E-2</v>
+      </c>
+      <c r="J3" s="160">
+        <v>2.1557406084288466E-2</v>
+      </c>
+      <c r="K3" s="160">
+        <v>7.0594945140186383E-2</v>
+      </c>
+      <c r="L3" s="160">
+        <v>-1.9000565067184283E-2</v>
+      </c>
+      <c r="M3" s="160">
+        <v>-9.1357418858191153E-3</v>
+      </c>
+      <c r="N3" s="160">
+        <v>-1.9620591031415557E-2</v>
+      </c>
+      <c r="O3" s="160">
+        <v>-1.9137456026697919E-2</v>
+      </c>
+      <c r="P3" s="160">
+        <v>-5.4122438277293128E-4</v>
+      </c>
+      <c r="Q3" s="160">
+        <v>2.1224584998035922E-2</v>
+      </c>
+      <c r="R3" s="160">
+        <v>1.6623080547468305E-2</v>
+      </c>
+      <c r="S3" s="160">
+        <v>5.118586777803813E-2</v>
+      </c>
+      <c r="T3" s="160">
+        <v>-87.046836493611409</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A4" s="160" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="160">
+        <v>-0.4197083426591271</v>
+      </c>
+      <c r="C4" s="160">
+        <v>-1.7935173747858028E-4</v>
+      </c>
+      <c r="D4" s="160">
+        <v>-0.27191717216847522</v>
+      </c>
+      <c r="E4" s="160">
+        <v>7.5949894164208942E-3</v>
+      </c>
+      <c r="F4" s="160">
+        <v>-7.748394861909369E-3</v>
+      </c>
+      <c r="G4" s="160">
+        <v>-2.6974709419077397E-4</v>
+      </c>
+      <c r="H4" s="160">
+        <v>-3.1088521687136494E-5</v>
+      </c>
+      <c r="I4" s="160">
+        <v>-5.9113763530178887E-4</v>
+      </c>
+      <c r="J4" s="160">
+        <v>-5.7466477529882765E-4</v>
+      </c>
+      <c r="K4" s="160">
+        <v>-1.9390266459817784E-3</v>
+      </c>
+      <c r="L4" s="160">
+        <v>5.2968759306815105E-4</v>
+      </c>
+      <c r="M4" s="160">
+        <v>2.5274137195274715E-4</v>
+      </c>
+      <c r="N4" s="160">
+        <v>5.4673144421557573E-4</v>
+      </c>
+      <c r="O4" s="160">
+        <v>5.3276086824871616E-4</v>
+      </c>
+      <c r="P4" s="160">
+        <v>1.5256245355421694E-5</v>
+      </c>
+      <c r="Q4" s="160">
+        <v>-5.9231019842059807E-4</v>
+      </c>
+      <c r="R4" s="160">
+        <v>-4.654526805825121E-4</v>
+      </c>
+      <c r="S4" s="160">
+        <v>-1.4285209877862304E-3</v>
+      </c>
+      <c r="T4" s="160">
+        <v>2.4310399428561311</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A5" s="160" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="160">
+        <v>0.43721588815505807</v>
+      </c>
+      <c r="C5" s="160">
+        <v>1.7502779710062803E-4</v>
+      </c>
+      <c r="D5" s="160">
+        <v>0.27734999427854845</v>
+      </c>
+      <c r="E5" s="160">
+        <v>-7.748394861909369E-3</v>
+      </c>
+      <c r="F5" s="160">
+        <v>7.9128744317976674E-3</v>
+      </c>
+      <c r="G5" s="160">
+        <v>2.7279596871876421E-4</v>
+      </c>
+      <c r="H5" s="160">
+        <v>3.0877978882473678E-5</v>
+      </c>
+      <c r="I5" s="160">
+        <v>5.4964401444143607E-4</v>
+      </c>
+      <c r="J5" s="160">
+        <v>4.848892933040222E-4</v>
+      </c>
+      <c r="K5" s="160">
+        <v>1.853184938339858E-3</v>
+      </c>
+      <c r="L5" s="160">
+        <v>-5.3464336690989267E-4</v>
+      </c>
+      <c r="M5" s="160">
+        <v>-2.4738017644410082E-4</v>
+      </c>
+      <c r="N5" s="160">
+        <v>-5.5033698257755947E-4</v>
+      </c>
+      <c r="O5" s="160">
+        <v>-5.3489948596596726E-4</v>
+      </c>
+      <c r="P5" s="160">
+        <v>-1.5254319953916795E-5</v>
+      </c>
+      <c r="Q5" s="160">
+        <v>6.0012374590046047E-4</v>
+      </c>
+      <c r="R5" s="160">
+        <v>4.7493387688168909E-4</v>
+      </c>
+      <c r="S5" s="160">
+        <v>1.4477968421635623E-3</v>
+      </c>
+      <c r="T5" s="160">
+        <v>-2.479003590669663</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A6" s="160" t="s">
+        <v>50</v>
+      </c>
+      <c r="B6" s="160">
+        <v>0.14467819555438441</v>
+      </c>
+      <c r="C6" s="160">
+        <v>6.1253561870731248E-5</v>
+      </c>
+      <c r="D6" s="160">
+        <v>9.8265176728999926E-3</v>
+      </c>
+      <c r="E6" s="160">
+        <v>-2.6974709419077397E-4</v>
+      </c>
+      <c r="F6" s="160">
+        <v>2.7279596871876421E-4</v>
+      </c>
+      <c r="G6" s="160">
+        <v>3.7278169803934931E-3</v>
+      </c>
+      <c r="H6" s="160">
+        <v>2.659026401547783E-5</v>
+      </c>
+      <c r="I6" s="160">
+        <v>1.1722493082651675E-4</v>
+      </c>
+      <c r="J6" s="160">
+        <v>9.6466856073054805E-5</v>
+      </c>
+      <c r="K6" s="160">
+        <v>5.184226175192555E-4</v>
+      </c>
+      <c r="L6" s="160">
+        <v>-2.4814970322100185E-4</v>
+      </c>
+      <c r="M6" s="160">
+        <v>-3.3863561613675826E-4</v>
+      </c>
+      <c r="N6" s="160">
+        <v>-3.1066739665635071E-4</v>
+      </c>
+      <c r="O6" s="160">
+        <v>-3.0885227243649879E-4</v>
+      </c>
+      <c r="P6" s="160">
+        <v>1.1101696040472994E-5</v>
+      </c>
+      <c r="Q6" s="160">
+        <v>3.2511657258515406E-4</v>
+      </c>
+      <c r="R6" s="160">
+        <v>3.0736558957823387E-4</v>
+      </c>
+      <c r="S6" s="160">
+        <v>8.6481007225365503E-4</v>
+      </c>
+      <c r="T6" s="160">
+        <v>-9.3247802460014739E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A7" s="160" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="160">
+        <v>-2.3369264226518048E-2</v>
+      </c>
+      <c r="C7" s="160">
+        <v>2.5886840098702005E-5</v>
+      </c>
+      <c r="D7" s="160">
+        <v>1.1317111183015705E-3</v>
+      </c>
+      <c r="E7" s="160">
+        <v>-3.1088521687136494E-5</v>
+      </c>
+      <c r="F7" s="160">
+        <v>3.0877978882473678E-5</v>
+      </c>
+      <c r="G7" s="160">
+        <v>2.659026401547783E-5</v>
+      </c>
+      <c r="H7" s="160">
+        <v>2.0351163580425743E-3</v>
+      </c>
+      <c r="I7" s="160">
+        <v>1.0795529786144797E-3</v>
+      </c>
+      <c r="J7" s="160">
+        <v>1.1039924478113495E-3</v>
+      </c>
+      <c r="K7" s="160">
+        <v>1.1342747272619154E-3</v>
+      </c>
+      <c r="L7" s="160">
+        <v>-1.1445369473061856E-5</v>
+      </c>
+      <c r="M7" s="160">
+        <v>-8.2117605647798989E-5</v>
+      </c>
+      <c r="N7" s="160">
+        <v>4.1083429444412458E-5</v>
+      </c>
+      <c r="O7" s="160">
+        <v>2.7828852219955336E-5</v>
+      </c>
+      <c r="P7" s="160">
+        <v>4.0958530735474242E-6</v>
+      </c>
+      <c r="Q7" s="160">
+        <v>-1.9953480612792777E-4</v>
+      </c>
+      <c r="R7" s="160">
+        <v>-4.9457960830362468E-5</v>
+      </c>
+      <c r="S7" s="160">
+        <v>3.1089157637864554E-5</v>
+      </c>
+      <c r="T7" s="160">
+        <v>-1.1484694951633068E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A8" s="160" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="160">
+        <v>1.5750477701682725E-2</v>
+      </c>
+      <c r="C8" s="160">
+        <v>1.7962333265363886E-4</v>
+      </c>
+      <c r="D8" s="160">
+        <v>2.1680501905967375E-2</v>
+      </c>
+      <c r="E8" s="160">
+        <v>-5.9113763530178887E-4</v>
+      </c>
+      <c r="F8" s="160">
+        <v>5.4964401444143607E-4</v>
+      </c>
+      <c r="G8" s="160">
+        <v>1.1722493082651675E-4</v>
+      </c>
+      <c r="H8" s="160">
+        <v>1.0795529786144797E-3</v>
+      </c>
+      <c r="I8" s="160">
+        <v>3.5191710524145221E-3</v>
+      </c>
+      <c r="J8" s="160">
+        <v>2.1603419780203909E-3</v>
+      </c>
+      <c r="K8" s="160">
+        <v>2.4913629538619725E-3</v>
+      </c>
+      <c r="L8" s="160">
+        <v>-2.0574618623507568E-4</v>
+      </c>
+      <c r="M8" s="160">
+        <v>-4.6566696754481857E-4</v>
+      </c>
+      <c r="N8" s="160">
+        <v>-2.4427045563542304E-4</v>
+      </c>
+      <c r="O8" s="160">
+        <v>-2.7975330527061498E-4</v>
+      </c>
+      <c r="P8" s="160">
+        <v>5.5651620878942321E-6</v>
+      </c>
+      <c r="Q8" s="160">
+        <v>-2.8675465336052905E-4</v>
+      </c>
+      <c r="R8" s="160">
+        <v>-1.9529016969008217E-4</v>
+      </c>
+      <c r="S8" s="160">
+        <v>9.331566768846361E-5</v>
+      </c>
+      <c r="T8" s="160">
+        <v>-0.20049545174530081</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A9" s="160" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="160">
+        <v>0.17301179530690947</v>
+      </c>
+      <c r="C9" s="160">
+        <v>5.3124240932293852E-5</v>
+      </c>
+      <c r="D9" s="160">
+        <v>2.1557406084288466E-2</v>
+      </c>
+      <c r="E9" s="160">
+        <v>-5.7466477529882765E-4</v>
+      </c>
+      <c r="F9" s="160">
+        <v>4.848892933040222E-4</v>
+      </c>
+      <c r="G9" s="160">
+        <v>9.6466856073054805E-5</v>
+      </c>
+      <c r="H9" s="160">
+        <v>1.1039924478113495E-3</v>
+      </c>
+      <c r="I9" s="160">
+        <v>2.1603419780203909E-3</v>
+      </c>
+      <c r="J9" s="160">
+        <v>6.8613120248816693E-3</v>
+      </c>
+      <c r="K9" s="160">
+        <v>3.5710211974613604E-3</v>
+      </c>
+      <c r="L9" s="160">
+        <v>-8.2101969672940256E-5</v>
+      </c>
+      <c r="M9" s="160">
+        <v>-4.3333568503225312E-4</v>
+      </c>
+      <c r="N9" s="160">
+        <v>-5.5710005043035915E-5</v>
+      </c>
+      <c r="O9" s="160">
+        <v>-1.6421080921541487E-4</v>
+      </c>
+      <c r="P9" s="160">
+        <v>3.6700923677513569E-5</v>
+      </c>
+      <c r="Q9" s="160">
+        <v>-3.6410049682397694E-4</v>
+      </c>
+      <c r="R9" s="160">
+        <v>-3.5729122436234384E-4</v>
+      </c>
+      <c r="S9" s="160">
+        <v>-1.0940982944834809E-4</v>
+      </c>
+      <c r="T9" s="160">
+        <v>-0.20493923900230726</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A10" s="160" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="160">
+        <v>7.6593048516463052E-3</v>
+      </c>
+      <c r="C10" s="160">
+        <v>4.5712785431306635E-4</v>
+      </c>
+      <c r="D10" s="160">
+        <v>7.0594945140186383E-2</v>
+      </c>
+      <c r="E10" s="160">
+        <v>-1.9390266459817784E-3</v>
+      </c>
+      <c r="F10" s="160">
+        <v>1.853184938339858E-3</v>
+      </c>
+      <c r="G10" s="160">
+        <v>5.184226175192555E-4</v>
+      </c>
+      <c r="H10" s="160">
+        <v>1.1342747272619154E-3</v>
+      </c>
+      <c r="I10" s="160">
+        <v>2.4913629538619725E-3</v>
+      </c>
+      <c r="J10" s="160">
+        <v>3.5710211974613604E-3</v>
+      </c>
+      <c r="K10" s="160">
+        <v>1.2413269736258559E-2</v>
+      </c>
+      <c r="L10" s="160">
+        <v>-8.7038479762639731E-4</v>
+      </c>
+      <c r="M10" s="160">
+        <v>-1.1726836768198232E-3</v>
+      </c>
+      <c r="N10" s="160">
+        <v>-9.3184417924073448E-4</v>
+      </c>
+      <c r="O10" s="160">
+        <v>-9.2702345163249433E-4</v>
+      </c>
+      <c r="P10" s="160">
+        <v>9.0255478899379377E-5</v>
+      </c>
+      <c r="Q10" s="160">
+        <v>-7.3917506518340892E-4</v>
+      </c>
+      <c r="R10" s="160">
+        <v>-6.8814491149582491E-4</v>
+      </c>
+      <c r="S10" s="160">
+        <v>5.4224701085513194E-4</v>
+      </c>
+      <c r="T10" s="160">
+        <v>-0.646249684580674</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A11" s="160" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" s="160">
+        <v>6.5097548678465608E-2</v>
+      </c>
+      <c r="C11" s="160">
+        <v>-1.6298682901668814E-4</v>
+      </c>
+      <c r="D11" s="160">
+        <v>-1.9000565067184283E-2</v>
+      </c>
+      <c r="E11" s="160">
+        <v>5.2968759306815105E-4</v>
+      </c>
+      <c r="F11" s="160">
+        <v>-5.3464336690989267E-4</v>
+      </c>
+      <c r="G11" s="160">
+        <v>-2.4814970322100185E-4</v>
+      </c>
+      <c r="H11" s="160">
+        <v>-1.1445369473061856E-5</v>
+      </c>
+      <c r="I11" s="160">
+        <v>-2.0574618623507568E-4</v>
+      </c>
+      <c r="J11" s="160">
+        <v>-8.2101969672940256E-5</v>
+      </c>
+      <c r="K11" s="160">
+        <v>-8.7038479762639731E-4</v>
+      </c>
+      <c r="L11" s="160">
+        <v>4.2735779692884279E-3</v>
+      </c>
+      <c r="M11" s="160">
+        <v>2.1727338564752341E-3</v>
+      </c>
+      <c r="N11" s="160">
+        <v>2.1377722098065571E-3</v>
+      </c>
+      <c r="O11" s="160">
+        <v>2.1529385102268522E-3</v>
+      </c>
+      <c r="P11" s="160">
+        <v>-5.0490534268104841E-5</v>
+      </c>
+      <c r="Q11" s="160">
+        <v>3.7546635326559091E-4</v>
+      </c>
+      <c r="R11" s="160">
+        <v>2.3073863273776613E-4</v>
+      </c>
+      <c r="S11" s="160">
+        <v>-1.3882236142254839E-4</v>
+      </c>
+      <c r="T11" s="160">
+        <v>0.16930219269720226</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A12" s="160" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" s="160">
+        <v>-8.500710866007391E-2</v>
+      </c>
+      <c r="C12" s="160">
+        <v>-1.5639961434307749E-4</v>
+      </c>
+      <c r="D12" s="160">
+        <v>-9.1357418858191153E-3</v>
+      </c>
+      <c r="E12" s="160">
+        <v>2.5274137195274715E-4</v>
+      </c>
+      <c r="F12" s="160">
+        <v>-2.4738017644410082E-4</v>
+      </c>
+      <c r="G12" s="160">
+        <v>-3.3863561613675826E-4</v>
+      </c>
+      <c r="H12" s="160">
+        <v>-8.2117605647798989E-5</v>
+      </c>
+      <c r="I12" s="160">
+        <v>-4.6566696754481857E-4</v>
+      </c>
+      <c r="J12" s="160">
+        <v>-4.3333568503225312E-4</v>
+      </c>
+      <c r="K12" s="160">
+        <v>-1.1726836768198232E-3</v>
+      </c>
+      <c r="L12" s="160">
+        <v>2.1727338564752341E-3</v>
+      </c>
+      <c r="M12" s="160">
+        <v>6.1623331386975733E-3</v>
+      </c>
+      <c r="N12" s="160">
+        <v>2.1765977228003393E-3</v>
+      </c>
+      <c r="O12" s="160">
+        <v>2.177473831481206E-3</v>
+      </c>
+      <c r="P12" s="160">
+        <v>-2.3288002807814526E-5</v>
+      </c>
+      <c r="Q12" s="160">
+        <v>4.4261816558893545E-4</v>
+      </c>
+      <c r="R12" s="160">
+        <v>4.9553427594065114E-5</v>
+      </c>
+      <c r="S12" s="160">
+        <v>-4.1974123642219904E-4</v>
+      </c>
+      <c r="T12" s="160">
+        <v>8.138237648560942E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A13" s="160" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" s="160">
+        <v>7.2288874385098692E-2</v>
+      </c>
+      <c r="C13" s="160">
+        <v>-1.8268489467859056E-4</v>
+      </c>
+      <c r="D13" s="160">
+        <v>-1.9620591031415557E-2</v>
+      </c>
+      <c r="E13" s="160">
+        <v>5.4673144421557573E-4</v>
+      </c>
+      <c r="F13" s="160">
+        <v>-5.5033698257755947E-4</v>
+      </c>
+      <c r="G13" s="160">
+        <v>-3.1066739665635071E-4</v>
+      </c>
+      <c r="H13" s="160">
+        <v>4.1083429444412458E-5</v>
+      </c>
+      <c r="I13" s="160">
+        <v>-2.4427045563542304E-4</v>
+      </c>
+      <c r="J13" s="160">
+        <v>-5.5710005043035915E-5</v>
+      </c>
+      <c r="K13" s="160">
+        <v>-9.3184417924073448E-4</v>
+      </c>
+      <c r="L13" s="160">
+        <v>2.1377722098065571E-3</v>
+      </c>
+      <c r="M13" s="160">
+        <v>2.1765977228003393E-3</v>
+      </c>
+      <c r="N13" s="160">
+        <v>4.2199736748816403E-3</v>
+      </c>
+      <c r="O13" s="160">
+        <v>2.1512558183306059E-3</v>
+      </c>
+      <c r="P13" s="160">
+        <v>-4.8662458668889425E-5</v>
+      </c>
+      <c r="Q13" s="160">
+        <v>2.107307716453094E-4</v>
+      </c>
+      <c r="R13" s="160">
+        <v>2.6193446674797893E-4</v>
+      </c>
+      <c r="S13" s="160">
+        <v>-2.231025684252437E-4</v>
+      </c>
+      <c r="T13" s="160">
+        <v>0.17498962450753375</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A14" s="160" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" s="160">
+        <v>0.10708255489603041</v>
+      </c>
+      <c r="C14" s="160">
+        <v>-1.9876794228678666E-4</v>
+      </c>
+      <c r="D14" s="160">
+        <v>-1.9137456026697919E-2</v>
+      </c>
+      <c r="E14" s="160">
+        <v>5.3276086824871616E-4</v>
+      </c>
+      <c r="F14" s="160">
+        <v>-5.3489948596596726E-4</v>
+      </c>
+      <c r="G14" s="160">
+        <v>-3.0885227243649879E-4</v>
+      </c>
+      <c r="H14" s="160">
+        <v>2.7828852219955336E-5</v>
+      </c>
+      <c r="I14" s="160">
+        <v>-2.7975330527061498E-4</v>
+      </c>
+      <c r="J14" s="160">
+        <v>-1.6421080921541487E-4</v>
+      </c>
+      <c r="K14" s="160">
+        <v>-9.2702345163249433E-4</v>
+      </c>
+      <c r="L14" s="160">
+        <v>2.1529385102268522E-3</v>
+      </c>
+      <c r="M14" s="160">
+        <v>2.177473831481206E-3</v>
+      </c>
+      <c r="N14" s="160">
+        <v>2.1512558183306059E-3</v>
+      </c>
+      <c r="O14" s="160">
+        <v>2.9671754321742606E-3</v>
+      </c>
+      <c r="P14" s="160">
+        <v>-3.1700049359660414E-5</v>
+      </c>
+      <c r="Q14" s="160">
+        <v>2.7034284619621794E-4</v>
+      </c>
+      <c r="R14" s="160">
+        <v>1.3839055425524105E-4</v>
+      </c>
+      <c r="S14" s="160">
+        <v>-2.3364827636957429E-4</v>
+      </c>
+      <c r="T14" s="160">
+        <v>0.1705773542758573</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A15" s="160" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" s="160">
+        <v>-4.3956279406245483E-2</v>
+      </c>
+      <c r="C15" s="160">
+        <v>-2.5926383840036912E-6</v>
+      </c>
+      <c r="D15" s="160">
+        <v>-5.4122438277293128E-4</v>
+      </c>
+      <c r="E15" s="160">
+        <v>1.5256245355421694E-5</v>
+      </c>
+      <c r="F15" s="160">
+        <v>-1.5254319953916795E-5</v>
+      </c>
+      <c r="G15" s="160">
+        <v>1.1101696040472994E-5</v>
+      </c>
+      <c r="H15" s="160">
+        <v>4.0958530735474242E-6</v>
+      </c>
+      <c r="I15" s="160">
+        <v>5.5651620878942321E-6</v>
+      </c>
+      <c r="J15" s="160">
+        <v>3.6700923677513569E-5</v>
+      </c>
+      <c r="K15" s="160">
+        <v>9.0255478899379377E-5</v>
+      </c>
+      <c r="L15" s="160">
+        <v>-5.0490534268104841E-5</v>
+      </c>
+      <c r="M15" s="160">
+        <v>-2.3288002807814526E-5</v>
+      </c>
+      <c r="N15" s="160">
+        <v>-4.8662458668889425E-5</v>
+      </c>
+      <c r="O15" s="160">
+        <v>-3.1700049359660414E-5</v>
+      </c>
+      <c r="P15" s="160">
+        <v>1.0450098799204517E-4</v>
+      </c>
+      <c r="Q15" s="160">
+        <v>-5.296389939898657E-4</v>
+      </c>
+      <c r="R15" s="160">
+        <v>-6.350648985401253E-4</v>
+      </c>
+      <c r="S15" s="160">
+        <v>-7.7643294212445633E-4</v>
+      </c>
+      <c r="T15" s="160">
+        <v>3.2276316274895255E-3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A16" s="160" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16" s="160">
+        <v>2.6332702114646726E-2</v>
+      </c>
+      <c r="C16" s="160">
+        <v>-6.3352423641038942E-5</v>
+      </c>
+      <c r="D16" s="160">
+        <v>2.1224584998035922E-2</v>
+      </c>
+      <c r="E16" s="160">
+        <v>-5.9231019842059807E-4</v>
+      </c>
+      <c r="F16" s="160">
+        <v>6.0012374590046047E-4</v>
+      </c>
+      <c r="G16" s="160">
+        <v>3.2511657258515406E-4</v>
+      </c>
+      <c r="H16" s="160">
+        <v>-1.9953480612792777E-4</v>
+      </c>
+      <c r="I16" s="160">
+        <v>-2.8675465336052905E-4</v>
+      </c>
+      <c r="J16" s="160">
+        <v>-3.6410049682397694E-4</v>
+      </c>
+      <c r="K16" s="160">
+        <v>-7.3917506518340892E-4</v>
+      </c>
+      <c r="L16" s="160">
+        <v>3.7546635326559091E-4</v>
+      </c>
+      <c r="M16" s="160">
+        <v>4.4261816558893545E-4</v>
+      </c>
+      <c r="N16" s="160">
+        <v>2.107307716453094E-4</v>
+      </c>
+      <c r="O16" s="160">
+        <v>2.7034284619621794E-4</v>
+      </c>
+      <c r="P16" s="160">
+        <v>-5.296389939898657E-4</v>
+      </c>
+      <c r="Q16" s="160">
+        <v>8.4108387304427309E-3</v>
+      </c>
+      <c r="R16" s="160">
+        <v>3.7452771418665723E-3</v>
+      </c>
+      <c r="S16" s="160">
+        <v>4.4637701643416103E-3</v>
+      </c>
+      <c r="T16" s="160">
+        <v>-0.18279497533811107</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A17" s="160" t="s">
+        <v>30</v>
+      </c>
+      <c r="B17" s="160">
+        <v>0.53333941696302101</v>
+      </c>
+      <c r="C17" s="160">
+        <v>-2.1740147754592543E-5</v>
+      </c>
+      <c r="D17" s="160">
+        <v>1.6623080547468305E-2</v>
+      </c>
+      <c r="E17" s="160">
+        <v>-4.654526805825121E-4</v>
+      </c>
+      <c r="F17" s="160">
+        <v>4.7493387688168909E-4</v>
+      </c>
+      <c r="G17" s="160">
+        <v>3.0736558957823387E-4</v>
+      </c>
+      <c r="H17" s="160">
+        <v>-4.9457960830362468E-5</v>
+      </c>
+      <c r="I17" s="160">
+        <v>-1.9529016969008217E-4</v>
+      </c>
+      <c r="J17" s="160">
+        <v>-3.5729122436234384E-4</v>
+      </c>
+      <c r="K17" s="160">
+        <v>-6.8814491149582491E-4</v>
+      </c>
+      <c r="L17" s="160">
+        <v>2.3073863273776613E-4</v>
+      </c>
+      <c r="M17" s="160">
+        <v>4.9553427594065114E-5</v>
+      </c>
+      <c r="N17" s="160">
+        <v>2.6193446674797893E-4</v>
+      </c>
+      <c r="O17" s="160">
+        <v>1.3839055425524105E-4</v>
+      </c>
+      <c r="P17" s="160">
+        <v>-6.350648985401253E-4</v>
+      </c>
+      <c r="Q17" s="160">
+        <v>3.7452771418665723E-3</v>
+      </c>
+      <c r="R17" s="160">
+        <v>7.458475416199737E-3</v>
+      </c>
+      <c r="S17" s="160">
+        <v>5.297380986711374E-3</v>
+      </c>
+      <c r="T17" s="160">
+        <v>-0.13942380418630584</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A18" s="160" t="s">
+        <v>31</v>
+      </c>
+      <c r="B18" s="160">
+        <v>0.57490883290859818</v>
+      </c>
+      <c r="C18" s="160">
+        <v>2.0931814563870769E-4</v>
+      </c>
+      <c r="D18" s="160">
+        <v>5.118586777803813E-2</v>
+      </c>
+      <c r="E18" s="160">
+        <v>-1.4285209877862304E-3</v>
+      </c>
+      <c r="F18" s="160">
+        <v>1.4477968421635623E-3</v>
+      </c>
+      <c r="G18" s="160">
+        <v>8.6481007225365503E-4</v>
+      </c>
+      <c r="H18" s="160">
+        <v>3.1089157637864554E-5</v>
+      </c>
+      <c r="I18" s="160">
+        <v>9.331566768846361E-5</v>
+      </c>
+      <c r="J18" s="160">
+        <v>-1.0940982944834809E-4</v>
+      </c>
+      <c r="K18" s="160">
+        <v>5.4224701085513194E-4</v>
+      </c>
+      <c r="L18" s="160">
+        <v>-1.3882236142254839E-4</v>
+      </c>
+      <c r="M18" s="160">
+        <v>-4.1974123642219904E-4</v>
+      </c>
+      <c r="N18" s="160">
+        <v>-2.231025684252437E-4</v>
+      </c>
+      <c r="O18" s="160">
+        <v>-2.3364827636957429E-4</v>
+      </c>
+      <c r="P18" s="160">
+        <v>-7.7643294212445633E-4</v>
+      </c>
+      <c r="Q18" s="160">
+        <v>4.4637701643416103E-3</v>
+      </c>
+      <c r="R18" s="160">
+        <v>5.297380986711374E-3</v>
+      </c>
+      <c r="S18" s="160">
+        <v>9.0068675290532318E-3</v>
+      </c>
+      <c r="T18" s="160">
+        <v>-0.4476073374168017</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A19" s="160" t="s">
+        <v>32</v>
+      </c>
+      <c r="B19" s="160">
+        <v>-128.71315026216749</v>
+      </c>
+      <c r="C19" s="160">
+        <v>-5.9911043825341848E-2</v>
+      </c>
+      <c r="D19" s="160">
+        <v>-87.046836493611409</v>
+      </c>
+      <c r="E19" s="160">
+        <v>2.4310399428561311</v>
+      </c>
+      <c r="F19" s="160">
+        <v>-2.479003590669663</v>
+      </c>
+      <c r="G19" s="160">
+        <v>-9.3247802460014739E-2</v>
+      </c>
+      <c r="H19" s="160">
+        <v>-1.1484694951633068E-2</v>
+      </c>
+      <c r="I19" s="160">
+        <v>-0.20049545174530081</v>
+      </c>
+      <c r="J19" s="160">
+        <v>-0.20493923900230726</v>
+      </c>
+      <c r="K19" s="160">
+        <v>-0.646249684580674</v>
+      </c>
+      <c r="L19" s="160">
+        <v>0.16930219269720226</v>
+      </c>
+      <c r="M19" s="160">
+        <v>8.138237648560942E-2</v>
+      </c>
+      <c r="N19" s="160">
+        <v>0.17498962450753375</v>
+      </c>
+      <c r="O19" s="160">
+        <v>0.1705773542758573</v>
+      </c>
+      <c r="P19" s="160">
+        <v>3.2276316274895255E-3</v>
+      </c>
+      <c r="Q19" s="160">
+        <v>-0.18279497533811107</v>
+      </c>
+      <c r="R19" s="160">
+        <v>-0.13942380418630584</v>
+      </c>
+      <c r="S19" s="160">
+        <v>-0.4476073374168017</v>
+      </c>
+      <c r="T19" s="160">
+        <v>778.37442023346375</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:T18"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:S18"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -5152,7 +6352,1084 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9686BA2-7B98-9640-9567-8119275CDCBD}">
+  <dimension ref="A1:S18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:S18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H1" t="s">
+        <v>41</v>
+      </c>
+      <c r="I1" t="s">
+        <v>42</v>
+      </c>
+      <c r="J1" t="s">
+        <v>43</v>
+      </c>
+      <c r="K1" t="s">
+        <v>44</v>
+      </c>
+      <c r="L1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M1" t="s">
+        <v>25</v>
+      </c>
+      <c r="N1" t="s">
+        <v>26</v>
+      </c>
+      <c r="O1" t="s">
+        <v>27</v>
+      </c>
+      <c r="P1" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>29</v>
+      </c>
+      <c r="R1" t="s">
+        <v>30</v>
+      </c>
+      <c r="S1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2">
+        <v>-0.2357257411749302</v>
+      </c>
+      <c r="C2">
+        <v>2.4510805113261143E-3</v>
+      </c>
+      <c r="D2">
+        <v>-3.2102615200586395E-5</v>
+      </c>
+      <c r="E2">
+        <v>3.5874943174665256E-7</v>
+      </c>
+      <c r="F2">
+        <v>1.3155040114384655E-3</v>
+      </c>
+      <c r="G2">
+        <v>7.0996839979951506E-4</v>
+      </c>
+      <c r="H2">
+        <v>-1.9479529407794363E-4</v>
+      </c>
+      <c r="I2">
+        <v>-3.0969184171741193E-5</v>
+      </c>
+      <c r="J2">
+        <v>2.1796671187530441E-4</v>
+      </c>
+      <c r="K2">
+        <v>-4.4968919297954551E-4</v>
+      </c>
+      <c r="L2">
+        <v>-1.134327996341339E-4</v>
+      </c>
+      <c r="M2">
+        <v>6.6915304259416455E-4</v>
+      </c>
+      <c r="N2">
+        <v>-3.5139446903519423E-5</v>
+      </c>
+      <c r="O2">
+        <v>4.1423720219982109E-5</v>
+      </c>
+      <c r="P2">
+        <v>1.5214341787043363E-5</v>
+      </c>
+      <c r="Q2">
+        <v>1.5659633116992151E-4</v>
+      </c>
+      <c r="R2">
+        <v>-2.0499464705725241E-4</v>
+      </c>
+      <c r="S2">
+        <v>-1.071861426878764E-3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3">
+        <v>-0.34007979569375091</v>
+      </c>
+      <c r="C3">
+        <v>-3.2102615200586395E-5</v>
+      </c>
+      <c r="D3">
+        <v>3.2668257938348359E-4</v>
+      </c>
+      <c r="E3">
+        <v>-3.3273899264722317E-6</v>
+      </c>
+      <c r="F3">
+        <v>-2.4993171956678322E-4</v>
+      </c>
+      <c r="G3">
+        <v>-5.5425458534225048E-4</v>
+      </c>
+      <c r="H3">
+        <v>6.9082493282138484E-5</v>
+      </c>
+      <c r="I3">
+        <v>2.6531395646011303E-4</v>
+      </c>
+      <c r="J3">
+        <v>-1.1053735200803108E-4</v>
+      </c>
+      <c r="K3">
+        <v>-3.209927813802721E-4</v>
+      </c>
+      <c r="L3">
+        <v>-3.1066795499443042E-6</v>
+      </c>
+      <c r="M3">
+        <v>-3.3805057277357803E-5</v>
+      </c>
+      <c r="N3">
+        <v>-5.3210728654050116E-5</v>
+      </c>
+      <c r="O3">
+        <v>-4.0588089215973298E-5</v>
+      </c>
+      <c r="P3">
+        <v>2.0150823963529922E-6</v>
+      </c>
+      <c r="Q3">
+        <v>-2.5388271398692468E-5</v>
+      </c>
+      <c r="R3">
+        <v>-1.3908125390932943E-4</v>
+      </c>
+      <c r="S3">
+        <v>-5.6876639238300653E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4">
+        <v>2.9543690733157659E-3</v>
+      </c>
+      <c r="C4">
+        <v>3.5874943174665256E-7</v>
+      </c>
+      <c r="D4">
+        <v>-3.3273899264722317E-6</v>
+      </c>
+      <c r="E4">
+        <v>3.5814620326587269E-8</v>
+      </c>
+      <c r="F4">
+        <v>3.1469412902748139E-6</v>
+      </c>
+      <c r="G4">
+        <v>5.1295736184548777E-6</v>
+      </c>
+      <c r="H4">
+        <v>-9.2823310216513826E-7</v>
+      </c>
+      <c r="I4">
+        <v>-2.4595860302240864E-6</v>
+      </c>
+      <c r="J4">
+        <v>2.8926138827916355E-6</v>
+      </c>
+      <c r="K4">
+        <v>7.8004654975365808E-7</v>
+      </c>
+      <c r="L4">
+        <v>1.7598418220390846E-7</v>
+      </c>
+      <c r="M4">
+        <v>-9.367871689660971E-8</v>
+      </c>
+      <c r="N4">
+        <v>5.3215542863501981E-7</v>
+      </c>
+      <c r="O4">
+        <v>7.208989607210281E-7</v>
+      </c>
+      <c r="P4">
+        <v>-4.6296400565728595E-8</v>
+      </c>
+      <c r="Q4">
+        <v>5.0923021267038342E-8</v>
+      </c>
+      <c r="R4">
+        <v>1.007662295913491E-6</v>
+      </c>
+      <c r="S4">
+        <v>5.7203814565399291E-5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B5">
+        <v>-0.27458673464211075</v>
+      </c>
+      <c r="C5">
+        <v>1.3155040114384655E-3</v>
+      </c>
+      <c r="D5">
+        <v>-2.4993171956678322E-4</v>
+      </c>
+      <c r="E5">
+        <v>3.1469412902748139E-6</v>
+      </c>
+      <c r="F5">
+        <v>1.3341010727619061E-2</v>
+      </c>
+      <c r="G5">
+        <v>1.2124283851861599E-3</v>
+      </c>
+      <c r="H5">
+        <v>5.5470433063515678E-4</v>
+      </c>
+      <c r="I5">
+        <v>-2.8825903313658312E-5</v>
+      </c>
+      <c r="J5">
+        <v>-1.3993518504160653E-3</v>
+      </c>
+      <c r="K5">
+        <v>-7.4421736770551861E-3</v>
+      </c>
+      <c r="L5">
+        <v>-2.9170164833557902E-4</v>
+      </c>
+      <c r="M5">
+        <v>5.2812495137603442E-4</v>
+      </c>
+      <c r="N5">
+        <v>2.711330067185766E-5</v>
+      </c>
+      <c r="O5">
+        <v>4.5553398609581909E-4</v>
+      </c>
+      <c r="P5">
+        <v>-4.7315589998412353E-5</v>
+      </c>
+      <c r="Q5">
+        <v>1.9194777633149158E-3</v>
+      </c>
+      <c r="R5">
+        <v>2.1916229380765807E-4</v>
+      </c>
+      <c r="S5">
+        <v>2.987005404224862E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B6">
+        <v>0.17925880173335171</v>
+      </c>
+      <c r="C6">
+        <v>7.0996839979951506E-4</v>
+      </c>
+      <c r="D6">
+        <v>-5.5425458534225048E-4</v>
+      </c>
+      <c r="E6">
+        <v>5.1295736184548777E-6</v>
+      </c>
+      <c r="F6">
+        <v>1.2124283851861599E-3</v>
+      </c>
+      <c r="G6">
+        <v>5.8011805879151874E-3</v>
+      </c>
+      <c r="H6">
+        <v>4.8234175505241329E-4</v>
+      </c>
+      <c r="I6">
+        <v>1.4116291766850023E-4</v>
+      </c>
+      <c r="J6">
+        <v>-1.168579199741789E-3</v>
+      </c>
+      <c r="K6">
+        <v>1.4779681656076113E-3</v>
+      </c>
+      <c r="L6">
+        <v>5.1987834106011124E-4</v>
+      </c>
+      <c r="M6">
+        <v>-4.0365845023471831E-4</v>
+      </c>
+      <c r="N6">
+        <v>-4.6885065709162377E-5</v>
+      </c>
+      <c r="O6">
+        <v>-2.3708002213186337E-4</v>
+      </c>
+      <c r="P6">
+        <v>-4.3756454070099492E-5</v>
+      </c>
+      <c r="Q6">
+        <v>8.9531589764649082E-4</v>
+      </c>
+      <c r="R6">
+        <v>3.0644237258910939E-4</v>
+      </c>
+      <c r="S6">
+        <v>9.0525163280049861E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B7">
+        <v>-6.9534422836427884E-2</v>
+      </c>
+      <c r="C7">
+        <v>-1.9479529407794363E-4</v>
+      </c>
+      <c r="D7">
+        <v>6.9082493282138484E-5</v>
+      </c>
+      <c r="E7">
+        <v>-9.2823310216513826E-7</v>
+      </c>
+      <c r="F7">
+        <v>5.5470433063515678E-4</v>
+      </c>
+      <c r="G7">
+        <v>4.8234175505241329E-4</v>
+      </c>
+      <c r="H7">
+        <v>3.5807792653095674E-3</v>
+      </c>
+      <c r="I7">
+        <v>-6.7006784962124119E-4</v>
+      </c>
+      <c r="J7">
+        <v>-2.5932068972744568E-4</v>
+      </c>
+      <c r="K7">
+        <v>5.3004827381918182E-4</v>
+      </c>
+      <c r="L7">
+        <v>-8.1454978769903813E-5</v>
+      </c>
+      <c r="M7">
+        <v>-7.0639979247848032E-4</v>
+      </c>
+      <c r="N7">
+        <v>-1.9179483533391463E-4</v>
+      </c>
+      <c r="O7">
+        <v>1.0127500121996744E-4</v>
+      </c>
+      <c r="P7">
+        <v>-1.7057921862689872E-5</v>
+      </c>
+      <c r="Q7">
+        <v>2.2669650910865408E-4</v>
+      </c>
+      <c r="R7">
+        <v>2.7234369031151539E-4</v>
+      </c>
+      <c r="S7">
+        <v>-1.1467843909237453E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>42</v>
+      </c>
+      <c r="B8">
+        <v>0.51150744318584307</v>
+      </c>
+      <c r="C8">
+        <v>-3.0969184171741193E-5</v>
+      </c>
+      <c r="D8">
+        <v>2.6531395646011303E-4</v>
+      </c>
+      <c r="E8">
+        <v>-2.4595860302240864E-6</v>
+      </c>
+      <c r="F8">
+        <v>-2.8825903313658312E-5</v>
+      </c>
+      <c r="G8">
+        <v>1.4116291766850023E-4</v>
+      </c>
+      <c r="H8">
+        <v>-6.7006784962124119E-4</v>
+      </c>
+      <c r="I8">
+        <v>2.7303054000252314E-3</v>
+      </c>
+      <c r="J8">
+        <v>4.154132725858256E-4</v>
+      </c>
+      <c r="K8">
+        <v>-1.7161018660371273E-3</v>
+      </c>
+      <c r="L8">
+        <v>-4.0512766380190064E-5</v>
+      </c>
+      <c r="M8">
+        <v>-2.900460207915824E-4</v>
+      </c>
+      <c r="N8">
+        <v>-3.8752395105443775E-5</v>
+      </c>
+      <c r="O8">
+        <v>-3.5063868238363583E-5</v>
+      </c>
+      <c r="P8">
+        <v>-4.0739932326283048E-6</v>
+      </c>
+      <c r="Q8">
+        <v>-3.3200711310977724E-5</v>
+      </c>
+      <c r="R8">
+        <v>3.1798894253409586E-4</v>
+      </c>
+      <c r="S8">
+        <v>-6.1935664974184495E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>43</v>
+      </c>
+      <c r="B9">
+        <v>-0.24635055290690239</v>
+      </c>
+      <c r="C9">
+        <v>2.1796671187530441E-4</v>
+      </c>
+      <c r="D9">
+        <v>-1.1053735200803108E-4</v>
+      </c>
+      <c r="E9">
+        <v>2.8926138827916355E-6</v>
+      </c>
+      <c r="F9">
+        <v>-1.3993518504160653E-3</v>
+      </c>
+      <c r="G9">
+        <v>-1.168579199741789E-3</v>
+      </c>
+      <c r="H9">
+        <v>-2.5932068972744568E-4</v>
+      </c>
+      <c r="I9">
+        <v>4.154132725858256E-4</v>
+      </c>
+      <c r="J9">
+        <v>1.3435035810614787E-2</v>
+      </c>
+      <c r="K9">
+        <v>-1.3368091534786512E-2</v>
+      </c>
+      <c r="L9">
+        <v>-3.6344722645133352E-4</v>
+      </c>
+      <c r="M9">
+        <v>-1.0901841361842706E-3</v>
+      </c>
+      <c r="N9">
+        <v>-3.3044424001780847E-4</v>
+      </c>
+      <c r="O9">
+        <v>-3.7290429401881154E-4</v>
+      </c>
+      <c r="P9">
+        <v>2.6312743073567753E-5</v>
+      </c>
+      <c r="Q9">
+        <v>-1.3255250684387709E-3</v>
+      </c>
+      <c r="R9">
+        <v>-8.3443871200859429E-4</v>
+      </c>
+      <c r="S9">
+        <v>5.9200936965700564E-4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>44</v>
+      </c>
+      <c r="B10">
+        <v>-9.1281211639630946E-2</v>
+      </c>
+      <c r="C10">
+        <v>-4.4968919297954551E-4</v>
+      </c>
+      <c r="D10">
+        <v>-3.209927813802721E-4</v>
+      </c>
+      <c r="E10">
+        <v>7.8004654975365808E-7</v>
+      </c>
+      <c r="F10">
+        <v>-7.4421736770551861E-3</v>
+      </c>
+      <c r="G10">
+        <v>1.4779681656076113E-3</v>
+      </c>
+      <c r="H10">
+        <v>5.3004827381918182E-4</v>
+      </c>
+      <c r="I10">
+        <v>-1.7161018660371273E-3</v>
+      </c>
+      <c r="J10">
+        <v>-1.3368091534786512E-2</v>
+      </c>
+      <c r="K10">
+        <v>3.4347191964421528E-2</v>
+      </c>
+      <c r="L10">
+        <v>4.5976563317379459E-4</v>
+      </c>
+      <c r="M10">
+        <v>5.6636045628112239E-4</v>
+      </c>
+      <c r="N10">
+        <v>1.0205902127152663E-4</v>
+      </c>
+      <c r="O10">
+        <v>5.650743794630616E-4</v>
+      </c>
+      <c r="P10">
+        <v>-4.7664987434007034E-5</v>
+      </c>
+      <c r="Q10">
+        <v>6.1369769975239575E-4</v>
+      </c>
+      <c r="R10">
+        <v>1.1007963247363136E-3</v>
+      </c>
+      <c r="S10">
+        <v>8.3346693516992681E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11">
+        <v>-6.8978290118414429E-2</v>
+      </c>
+      <c r="C11">
+        <v>-1.134327996341339E-4</v>
+      </c>
+      <c r="D11">
+        <v>-3.1066795499443042E-6</v>
+      </c>
+      <c r="E11">
+        <v>1.7598418220390846E-7</v>
+      </c>
+      <c r="F11">
+        <v>-2.9170164833557902E-4</v>
+      </c>
+      <c r="G11">
+        <v>5.1987834106011124E-4</v>
+      </c>
+      <c r="H11">
+        <v>-8.1454978769903813E-5</v>
+      </c>
+      <c r="I11">
+        <v>-4.0512766380190064E-5</v>
+      </c>
+      <c r="J11">
+        <v>-3.6344722645133352E-4</v>
+      </c>
+      <c r="K11">
+        <v>4.5976563317379459E-4</v>
+      </c>
+      <c r="L11">
+        <v>5.6395333464540178E-3</v>
+      </c>
+      <c r="M11">
+        <v>1.9227906617618608E-3</v>
+      </c>
+      <c r="N11">
+        <v>2.1182594171595954E-3</v>
+      </c>
+      <c r="O11">
+        <v>2.074201332245455E-3</v>
+      </c>
+      <c r="P11">
+        <v>-1.7242432668109032E-5</v>
+      </c>
+      <c r="Q11">
+        <v>3.8438426311568959E-5</v>
+      </c>
+      <c r="R11">
+        <v>2.9350108598232222E-5</v>
+      </c>
+      <c r="S11">
+        <v>-1.7788302096501749E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12">
+        <v>0.12108804698167266</v>
+      </c>
+      <c r="C12">
+        <v>6.6915304259416455E-4</v>
+      </c>
+      <c r="D12">
+        <v>-3.3805057277357803E-5</v>
+      </c>
+      <c r="E12">
+        <v>-9.367871689660971E-8</v>
+      </c>
+      <c r="F12">
+        <v>5.2812495137603442E-4</v>
+      </c>
+      <c r="G12">
+        <v>-4.0365845023471831E-4</v>
+      </c>
+      <c r="H12">
+        <v>-7.0639979247848032E-4</v>
+      </c>
+      <c r="I12">
+        <v>-2.900460207915824E-4</v>
+      </c>
+      <c r="J12">
+        <v>-1.0901841361842706E-3</v>
+      </c>
+      <c r="K12">
+        <v>5.6636045628112239E-4</v>
+      </c>
+      <c r="L12">
+        <v>1.9227906617618608E-3</v>
+      </c>
+      <c r="M12">
+        <v>1.1653267430124686E-2</v>
+      </c>
+      <c r="N12">
+        <v>2.0726025502786532E-3</v>
+      </c>
+      <c r="O12">
+        <v>1.9238334591054377E-3</v>
+      </c>
+      <c r="P12">
+        <v>2.6170587275969024E-4</v>
+      </c>
+      <c r="Q12">
+        <v>-1.2922142523765982E-3</v>
+      </c>
+      <c r="R12">
+        <v>-1.5817328532436495E-3</v>
+      </c>
+      <c r="S12">
+        <v>-5.3392843756465934E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13">
+        <v>-4.3533830844380367E-2</v>
+      </c>
+      <c r="C13">
+        <v>-3.5139446903519423E-5</v>
+      </c>
+      <c r="D13">
+        <v>-5.3210728654050116E-5</v>
+      </c>
+      <c r="E13">
+        <v>5.3215542863501981E-7</v>
+      </c>
+      <c r="F13">
+        <v>2.711330067185766E-5</v>
+      </c>
+      <c r="G13">
+        <v>-4.6885065709162377E-5</v>
+      </c>
+      <c r="H13">
+        <v>-1.9179483533391463E-4</v>
+      </c>
+      <c r="I13">
+        <v>-3.8752395105443775E-5</v>
+      </c>
+      <c r="J13">
+        <v>-3.3044424001780847E-4</v>
+      </c>
+      <c r="K13">
+        <v>1.0205902127152663E-4</v>
+      </c>
+      <c r="L13">
+        <v>2.1182594171595954E-3</v>
+      </c>
+      <c r="M13">
+        <v>2.0726025502786532E-3</v>
+      </c>
+      <c r="N13">
+        <v>5.6175928668167905E-3</v>
+      </c>
+      <c r="O13">
+        <v>2.1052134645858098E-3</v>
+      </c>
+      <c r="P13">
+        <v>-4.2811252519755954E-5</v>
+      </c>
+      <c r="Q13">
+        <v>1.2106338389784746E-4</v>
+      </c>
+      <c r="R13">
+        <v>1.0666779725571095E-4</v>
+      </c>
+      <c r="S13">
+        <v>-3.7854820042129765E-4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14">
+        <v>0.10555139221269344</v>
+      </c>
+      <c r="C14">
+        <v>4.1423720219982109E-5</v>
+      </c>
+      <c r="D14">
+        <v>-4.0588089215973298E-5</v>
+      </c>
+      <c r="E14">
+        <v>7.208989607210281E-7</v>
+      </c>
+      <c r="F14">
+        <v>4.5553398609581909E-4</v>
+      </c>
+      <c r="G14">
+        <v>-2.3708002213186337E-4</v>
+      </c>
+      <c r="H14">
+        <v>1.0127500121996744E-4</v>
+      </c>
+      <c r="I14">
+        <v>-3.5063868238363583E-5</v>
+      </c>
+      <c r="J14">
+        <v>-3.7290429401881154E-4</v>
+      </c>
+      <c r="K14">
+        <v>5.650743794630616E-4</v>
+      </c>
+      <c r="L14">
+        <v>2.074201332245455E-3</v>
+      </c>
+      <c r="M14">
+        <v>1.9238334591054377E-3</v>
+      </c>
+      <c r="N14">
+        <v>2.1052134645858098E-3</v>
+      </c>
+      <c r="O14">
+        <v>3.5621324567671297E-3</v>
+      </c>
+      <c r="P14">
+        <v>-4.7706700101161635E-5</v>
+      </c>
+      <c r="Q14">
+        <v>4.2981748317565664E-4</v>
+      </c>
+      <c r="R14">
+        <v>2.2117246711321771E-4</v>
+      </c>
+      <c r="S14">
+        <v>-8.1283515901022321E-4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15">
+        <v>3.6548479624977356E-2</v>
+      </c>
+      <c r="C15">
+        <v>1.5214341787043363E-5</v>
+      </c>
+      <c r="D15">
+        <v>2.0150823963529922E-6</v>
+      </c>
+      <c r="E15">
+        <v>-4.6296400565728595E-8</v>
+      </c>
+      <c r="F15">
+        <v>-4.7315589998412353E-5</v>
+      </c>
+      <c r="G15">
+        <v>-4.3756454070099492E-5</v>
+      </c>
+      <c r="H15">
+        <v>-1.7057921862689872E-5</v>
+      </c>
+      <c r="I15">
+        <v>-4.0739932326283048E-6</v>
+      </c>
+      <c r="J15">
+        <v>2.6312743073567753E-5</v>
+      </c>
+      <c r="K15">
+        <v>-4.7664987434007034E-5</v>
+      </c>
+      <c r="L15">
+        <v>-1.7242432668109032E-5</v>
+      </c>
+      <c r="M15">
+        <v>2.6170587275969024E-4</v>
+      </c>
+      <c r="N15">
+        <v>-4.2811252519755954E-5</v>
+      </c>
+      <c r="O15">
+        <v>-4.7706700101161635E-5</v>
+      </c>
+      <c r="P15">
+        <v>7.0177274632341786E-5</v>
+      </c>
+      <c r="Q15">
+        <v>-2.9327685974025357E-4</v>
+      </c>
+      <c r="R15">
+        <v>-3.5523627471954614E-4</v>
+      </c>
+      <c r="S15">
+        <v>-1.1145026544314017E-3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16">
+        <v>4.3470989796039826E-2</v>
+      </c>
+      <c r="C16">
+        <v>1.5659633116992151E-4</v>
+      </c>
+      <c r="D16">
+        <v>-2.5388271398692468E-5</v>
+      </c>
+      <c r="E16">
+        <v>5.0923021267038342E-8</v>
+      </c>
+      <c r="F16">
+        <v>1.9194777633149158E-3</v>
+      </c>
+      <c r="G16">
+        <v>8.9531589764649082E-4</v>
+      </c>
+      <c r="H16">
+        <v>2.2669650910865408E-4</v>
+      </c>
+      <c r="I16">
+        <v>-3.3200711310977724E-5</v>
+      </c>
+      <c r="J16">
+        <v>-1.3255250684387709E-3</v>
+      </c>
+      <c r="K16">
+        <v>6.1369769975239575E-4</v>
+      </c>
+      <c r="L16">
+        <v>3.8438426311568959E-5</v>
+      </c>
+      <c r="M16">
+        <v>-1.2922142523765982E-3</v>
+      </c>
+      <c r="N16">
+        <v>1.2106338389784746E-4</v>
+      </c>
+      <c r="O16">
+        <v>4.2981748317565664E-4</v>
+      </c>
+      <c r="P16">
+        <v>-2.9327685974025357E-4</v>
+      </c>
+      <c r="Q16">
+        <v>7.740807011377541E-3</v>
+      </c>
+      <c r="R16">
+        <v>2.1533847192886603E-3</v>
+      </c>
+      <c r="S16">
+        <v>4.0662015547679002E-3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>30</v>
+      </c>
+      <c r="B17">
+        <v>0.53628196671751027</v>
+      </c>
+      <c r="C17">
+        <v>-2.0499464705725241E-4</v>
+      </c>
+      <c r="D17">
+        <v>-1.3908125390932943E-4</v>
+      </c>
+      <c r="E17">
+        <v>1.007662295913491E-6</v>
+      </c>
+      <c r="F17">
+        <v>2.1916229380765807E-4</v>
+      </c>
+      <c r="G17">
+        <v>3.0644237258910939E-4</v>
+      </c>
+      <c r="H17">
+        <v>2.7234369031151539E-4</v>
+      </c>
+      <c r="I17">
+        <v>3.1798894253409586E-4</v>
+      </c>
+      <c r="J17">
+        <v>-8.3443871200859429E-4</v>
+      </c>
+      <c r="K17">
+        <v>1.1007963247363136E-3</v>
+      </c>
+      <c r="L17">
+        <v>2.9350108598232222E-5</v>
+      </c>
+      <c r="M17">
+        <v>-1.5817328532436495E-3</v>
+      </c>
+      <c r="N17">
+        <v>1.0666779725571095E-4</v>
+      </c>
+      <c r="O17">
+        <v>2.2117246711321771E-4</v>
+      </c>
+      <c r="P17">
+        <v>-3.5523627471954614E-4</v>
+      </c>
+      <c r="Q17">
+        <v>2.1533847192886603E-3</v>
+      </c>
+      <c r="R17">
+        <v>5.4761336869581009E-3</v>
+      </c>
+      <c r="S17">
+        <v>7.3056294348148943E-3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>32</v>
+      </c>
+      <c r="B18">
+        <v>3.8540519391474746</v>
+      </c>
+      <c r="C18">
+        <v>-1.071861426878764E-3</v>
+      </c>
+      <c r="D18">
+        <v>-5.6876639238300653E-3</v>
+      </c>
+      <c r="E18">
+        <v>5.7203814565399291E-5</v>
+      </c>
+      <c r="F18">
+        <v>2.987005404224862E-3</v>
+      </c>
+      <c r="G18">
+        <v>9.0525163280049861E-3</v>
+      </c>
+      <c r="H18">
+        <v>-1.1467843909237453E-3</v>
+      </c>
+      <c r="I18">
+        <v>-6.1935664974184495E-3</v>
+      </c>
+      <c r="J18">
+        <v>5.9200936965700564E-4</v>
+      </c>
+      <c r="K18">
+        <v>8.3346693516992681E-3</v>
+      </c>
+      <c r="L18">
+        <v>-1.7788302096501749E-3</v>
+      </c>
+      <c r="M18">
+        <v>-5.3392843756465934E-3</v>
+      </c>
+      <c r="N18">
+        <v>-3.7854820042129765E-4</v>
+      </c>
+      <c r="O18">
+        <v>-8.1283515901022321E-4</v>
+      </c>
+      <c r="P18">
+        <v>-1.1145026544314017E-3</v>
+      </c>
+      <c r="Q18">
+        <v>4.0662015547679002E-3</v>
+      </c>
+      <c r="R18">
+        <v>7.3056294348148943E-3</v>
+      </c>
+      <c r="S18">
+        <v>0.12060423355951824</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:C37"/>
   <sheetViews>
@@ -5572,11 +7849,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:V20"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="U20" sqref="A1:U20"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -6886,4 +9165,1319 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A5F786D-862E-7D46-A3AB-76063D2DED95}">
+  <dimension ref="A1:U20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P11" sqref="A1:U20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A1" s="161" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="161" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="160" t="s">
+        <v>62</v>
+      </c>
+      <c r="D1" s="160" t="s">
+        <v>63</v>
+      </c>
+      <c r="E1" s="160" t="s">
+        <v>64</v>
+      </c>
+      <c r="F1" s="160" t="s">
+        <v>65</v>
+      </c>
+      <c r="G1" s="160" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1" s="160" t="s">
+        <v>67</v>
+      </c>
+      <c r="I1" s="160" t="s">
+        <v>68</v>
+      </c>
+      <c r="J1" s="160" t="s">
+        <v>69</v>
+      </c>
+      <c r="K1" s="160" t="s">
+        <v>70</v>
+      </c>
+      <c r="L1" s="160" t="s">
+        <v>71</v>
+      </c>
+      <c r="M1" s="160" t="s">
+        <v>72</v>
+      </c>
+      <c r="N1" s="160" t="s">
+        <v>73</v>
+      </c>
+      <c r="O1" s="160" t="s">
+        <v>74</v>
+      </c>
+      <c r="P1" s="160" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q1" s="160" t="s">
+        <v>76</v>
+      </c>
+      <c r="R1" s="160" t="s">
+        <v>77</v>
+      </c>
+      <c r="S1" s="160" t="s">
+        <v>78</v>
+      </c>
+      <c r="T1" s="160" t="s">
+        <v>79</v>
+      </c>
+      <c r="U1" s="160" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A2" s="161" t="s">
+        <v>62</v>
+      </c>
+      <c r="B2" s="161">
+        <v>-0.1851331107411095</v>
+      </c>
+      <c r="C2" s="160">
+        <v>2.5990437235309794E-2</v>
+      </c>
+      <c r="D2" s="160">
+        <v>-9.270221380480774E-3</v>
+      </c>
+      <c r="E2" s="160">
+        <v>2.0676244320437165E-4</v>
+      </c>
+      <c r="F2" s="160">
+        <v>2.5610268186623875E-3</v>
+      </c>
+      <c r="G2" s="160">
+        <v>-2.3629843003578777E-3</v>
+      </c>
+      <c r="H2" s="160">
+        <v>-2.7329455358785799E-3</v>
+      </c>
+      <c r="I2" s="160">
+        <v>-5.4723802114532106E-3</v>
+      </c>
+      <c r="J2" s="160">
+        <v>-2.2496673757599647E-3</v>
+      </c>
+      <c r="K2" s="160">
+        <v>-1.337126851430994E-5</v>
+      </c>
+      <c r="L2" s="160">
+        <v>-2.1891856823406438E-3</v>
+      </c>
+      <c r="M2" s="160">
+        <v>5.6669764918504048E-5</v>
+      </c>
+      <c r="N2" s="160">
+        <v>5.1510873478297331E-4</v>
+      </c>
+      <c r="O2" s="160">
+        <v>8.7880342538172257E-2</v>
+      </c>
+      <c r="P2" s="160">
+        <v>1.439055119746919E-3</v>
+      </c>
+      <c r="Q2" s="160">
+        <v>-4.0689315322597159E-4</v>
+      </c>
+      <c r="R2" s="160">
+        <v>1.110339955305822E-5</v>
+      </c>
+      <c r="S2" s="160">
+        <v>-1.4701051190887156E-3</v>
+      </c>
+      <c r="T2" s="160">
+        <v>-9.1701749141058345E-4</v>
+      </c>
+      <c r="U2" s="160">
+        <v>1.8946138227211688E-3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A3" s="161" t="s">
+        <v>63</v>
+      </c>
+      <c r="B3" s="161">
+        <v>2.4984242443644855</v>
+      </c>
+      <c r="C3" s="160">
+        <v>-9.270221380480774E-3</v>
+      </c>
+      <c r="D3" s="160">
+        <v>0.1227972616109671</v>
+      </c>
+      <c r="E3" s="160">
+        <v>-2.5879401567409665E-3</v>
+      </c>
+      <c r="F3" s="160">
+        <v>-1.0325557511284394E-2</v>
+      </c>
+      <c r="G3" s="160">
+        <v>5.354110151501619E-3</v>
+      </c>
+      <c r="H3" s="160">
+        <v>4.7926738914170208E-3</v>
+      </c>
+      <c r="I3" s="160">
+        <v>7.4458051116920408E-3</v>
+      </c>
+      <c r="J3" s="160">
+        <v>6.637201667696809E-3</v>
+      </c>
+      <c r="K3" s="160">
+        <v>1.3334274550695201E-4</v>
+      </c>
+      <c r="L3" s="160">
+        <v>7.791539839853822E-4</v>
+      </c>
+      <c r="M3" s="160">
+        <v>-9.0173638339487092E-3</v>
+      </c>
+      <c r="N3" s="160">
+        <v>-2.0242235946012235E-2</v>
+      </c>
+      <c r="O3" s="160">
+        <v>-1.3986035022020817</v>
+      </c>
+      <c r="P3" s="160">
+        <v>1.8470049044626933E-3</v>
+      </c>
+      <c r="Q3" s="160">
+        <v>0.10415682330628889</v>
+      </c>
+      <c r="R3" s="160">
+        <v>-2.1698494664189475E-3</v>
+      </c>
+      <c r="S3" s="160">
+        <v>6.5100352188719188E-3</v>
+      </c>
+      <c r="T3" s="160">
+        <v>4.4845659265097667E-3</v>
+      </c>
+      <c r="U3" s="160">
+        <v>-1.2407128942348631</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A4" s="161" t="s">
+        <v>64</v>
+      </c>
+      <c r="B4" s="161">
+        <v>-4.1088662035675586E-2</v>
+      </c>
+      <c r="C4" s="160">
+        <v>2.0676244320437165E-4</v>
+      </c>
+      <c r="D4" s="160">
+        <v>-2.5879401567409665E-3</v>
+      </c>
+      <c r="E4" s="160">
+        <v>5.5363376822358187E-5</v>
+      </c>
+      <c r="F4" s="160">
+        <v>3.0394921209656381E-4</v>
+      </c>
+      <c r="G4" s="160">
+        <v>-9.5871193421933002E-5</v>
+      </c>
+      <c r="H4" s="160">
+        <v>-1.2787310608692969E-4</v>
+      </c>
+      <c r="I4" s="160">
+        <v>-1.3232150992742314E-4</v>
+      </c>
+      <c r="J4" s="160">
+        <v>-1.2973259780777705E-4</v>
+      </c>
+      <c r="K4" s="160">
+        <v>-2.0235229055515656E-6</v>
+      </c>
+      <c r="L4" s="160">
+        <v>-3.7146698134853394E-5</v>
+      </c>
+      <c r="M4" s="160">
+        <v>1.8057494798948739E-4</v>
+      </c>
+      <c r="N4" s="160">
+        <v>4.6870459206550439E-4</v>
+      </c>
+      <c r="O4" s="160">
+        <v>2.9040910348742736E-2</v>
+      </c>
+      <c r="P4" s="160">
+        <v>-4.7722422693127043E-5</v>
+      </c>
+      <c r="Q4" s="160">
+        <v>-2.5784274725718743E-3</v>
+      </c>
+      <c r="R4" s="160">
+        <v>5.3843878149397985E-5</v>
+      </c>
+      <c r="S4" s="160">
+        <v>-1.5651390419824432E-4</v>
+      </c>
+      <c r="T4" s="160">
+        <v>-1.2029668913989115E-4</v>
+      </c>
+      <c r="U4" s="160">
+        <v>3.0597157804174015E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A5" s="161" t="s">
+        <v>65</v>
+      </c>
+      <c r="B5" s="161">
+        <v>0.67263569508066245</v>
+      </c>
+      <c r="C5" s="160">
+        <v>2.5610268186623875E-3</v>
+      </c>
+      <c r="D5" s="160">
+        <v>-1.0325557511284394E-2</v>
+      </c>
+      <c r="E5" s="160">
+        <v>3.0394921209656381E-4</v>
+      </c>
+      <c r="F5" s="160">
+        <v>4.934422073214547E-2</v>
+      </c>
+      <c r="G5" s="160">
+        <v>-1.5035119786934452E-3</v>
+      </c>
+      <c r="H5" s="160">
+        <v>-6.1628837960936399E-3</v>
+      </c>
+      <c r="I5" s="160">
+        <v>-1.1948571120089164E-3</v>
+      </c>
+      <c r="J5" s="160">
+        <v>-6.1469074235460568E-3</v>
+      </c>
+      <c r="K5" s="160">
+        <v>6.9025246257722612E-4</v>
+      </c>
+      <c r="L5" s="160">
+        <v>-4.7981931064700941E-3</v>
+      </c>
+      <c r="M5" s="160">
+        <v>3.0743777002507147E-3</v>
+      </c>
+      <c r="N5" s="160">
+        <v>1.016704010825858E-2</v>
+      </c>
+      <c r="O5" s="160">
+        <v>2.9830211602031587E-2</v>
+      </c>
+      <c r="P5" s="160">
+        <v>4.8554709112269435E-3</v>
+      </c>
+      <c r="Q5" s="160">
+        <v>-4.9467139915576913E-2</v>
+      </c>
+      <c r="R5" s="160">
+        <v>1.0553442399555634E-3</v>
+      </c>
+      <c r="S5" s="160">
+        <v>-7.2055629481296447E-3</v>
+      </c>
+      <c r="T5" s="160">
+        <v>-6.0152523808594633E-3</v>
+      </c>
+      <c r="U5" s="160">
+        <v>0.52650696178581669</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A6" s="161" t="s">
+        <v>66</v>
+      </c>
+      <c r="B6" s="161">
+        <v>0.1274911429791776</v>
+      </c>
+      <c r="C6" s="160">
+        <v>-2.3629843003578777E-3</v>
+      </c>
+      <c r="D6" s="160">
+        <v>5.354110151501619E-3</v>
+      </c>
+      <c r="E6" s="160">
+        <v>-9.5871193421933002E-5</v>
+      </c>
+      <c r="F6" s="160">
+        <v>-1.5035119786934452E-3</v>
+      </c>
+      <c r="G6" s="160">
+        <v>4.486122447772347E-2</v>
+      </c>
+      <c r="H6" s="160">
+        <v>2.2478738526618556E-2</v>
+      </c>
+      <c r="I6" s="160">
+        <v>2.2099807751463824E-2</v>
+      </c>
+      <c r="J6" s="160">
+        <v>2.2110525732097177E-2</v>
+      </c>
+      <c r="K6" s="160">
+        <v>-8.1411571659570792E-5</v>
+      </c>
+      <c r="L6" s="160">
+        <v>-3.025506512017077E-3</v>
+      </c>
+      <c r="M6" s="160">
+        <v>-4.7033628432151843E-3</v>
+      </c>
+      <c r="N6" s="160">
+        <v>3.0933175404866051E-3</v>
+      </c>
+      <c r="O6" s="160">
+        <v>-8.5386238867528275E-2</v>
+      </c>
+      <c r="P6" s="160">
+        <v>-2.8873970464742861E-3</v>
+      </c>
+      <c r="Q6" s="160">
+        <v>-2.3387825911462767E-2</v>
+      </c>
+      <c r="R6" s="160">
+        <v>4.7286609447689046E-4</v>
+      </c>
+      <c r="S6" s="160">
+        <v>2.3369530589833973E-2</v>
+      </c>
+      <c r="T6" s="160">
+        <v>2.4267537119822602E-2</v>
+      </c>
+      <c r="U6" s="160">
+        <v>0.26789795838039099</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A7" s="161" t="s">
+        <v>67</v>
+      </c>
+      <c r="B7" s="161">
+        <v>-0.21030082937074854</v>
+      </c>
+      <c r="C7" s="160">
+        <v>-2.7329455358785799E-3</v>
+      </c>
+      <c r="D7" s="160">
+        <v>4.7926738914170208E-3</v>
+      </c>
+      <c r="E7" s="160">
+        <v>-1.2787310608692969E-4</v>
+      </c>
+      <c r="F7" s="160">
+        <v>-6.1628837960936399E-3</v>
+      </c>
+      <c r="G7" s="160">
+        <v>2.2478738526618556E-2</v>
+      </c>
+      <c r="H7" s="160">
+        <v>5.728414081248169E-2</v>
+      </c>
+      <c r="I7" s="160">
+        <v>2.4463697754624848E-2</v>
+      </c>
+      <c r="J7" s="160">
+        <v>2.5176490870686498E-2</v>
+      </c>
+      <c r="K7" s="160">
+        <v>-7.311322364202729E-5</v>
+      </c>
+      <c r="L7" s="160">
+        <v>1.3964214578385432E-3</v>
+      </c>
+      <c r="M7" s="160">
+        <v>-6.4555702985388879E-3</v>
+      </c>
+      <c r="N7" s="160">
+        <v>-4.5476122960031E-3</v>
+      </c>
+      <c r="O7" s="160">
+        <v>-5.9647244943152766E-2</v>
+      </c>
+      <c r="P7" s="160">
+        <v>-5.5379760447134187E-3</v>
+      </c>
+      <c r="Q7" s="160">
+        <v>2.6798582470341507E-2</v>
+      </c>
+      <c r="R7" s="160">
+        <v>-5.7113880525171763E-4</v>
+      </c>
+      <c r="S7" s="160">
+        <v>2.1644665590256369E-2</v>
+      </c>
+      <c r="T7" s="160">
+        <v>2.2575139577819744E-2</v>
+      </c>
+      <c r="U7" s="160">
+        <v>-0.32507577205139465</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A8" s="161" t="s">
+        <v>68</v>
+      </c>
+      <c r="B8" s="161">
+        <v>0.25078173801816778</v>
+      </c>
+      <c r="C8" s="160">
+        <v>-5.4723802114532106E-3</v>
+      </c>
+      <c r="D8" s="160">
+        <v>7.4458051116920408E-3</v>
+      </c>
+      <c r="E8" s="160">
+        <v>-1.3232150992742314E-4</v>
+      </c>
+      <c r="F8" s="160">
+        <v>-1.1948571120089164E-3</v>
+      </c>
+      <c r="G8" s="160">
+        <v>2.2099807751463824E-2</v>
+      </c>
+      <c r="H8" s="160">
+        <v>2.4463697754624848E-2</v>
+      </c>
+      <c r="I8" s="160">
+        <v>5.3673365345003443E-2</v>
+      </c>
+      <c r="J8" s="160">
+        <v>2.7063015906224241E-2</v>
+      </c>
+      <c r="K8" s="160">
+        <v>-2.015476968341757E-4</v>
+      </c>
+      <c r="L8" s="160">
+        <v>-1.7655392515956124E-4</v>
+      </c>
+      <c r="M8" s="160">
+        <v>-2.6172577357264108E-3</v>
+      </c>
+      <c r="N8" s="160">
+        <v>2.4354976656682545E-3</v>
+      </c>
+      <c r="O8" s="160">
+        <v>-0.11441747715922801</v>
+      </c>
+      <c r="P8" s="160">
+        <v>-2.407540674298457E-3</v>
+      </c>
+      <c r="Q8" s="160">
+        <v>3.5110494572182099E-3</v>
+      </c>
+      <c r="R8" s="160">
+        <v>-7.5253787542500675E-5</v>
+      </c>
+      <c r="S8" s="160">
+        <v>1.6366262480138026E-2</v>
+      </c>
+      <c r="T8" s="160">
+        <v>1.5769792226923096E-2</v>
+      </c>
+      <c r="U8" s="160">
+        <v>-5.0233387354936598E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A9" s="161" t="s">
+        <v>69</v>
+      </c>
+      <c r="B9" s="161">
+        <v>0.76884784757909441</v>
+      </c>
+      <c r="C9" s="160">
+        <v>-2.2496673757599647E-3</v>
+      </c>
+      <c r="D9" s="160">
+        <v>6.637201667696809E-3</v>
+      </c>
+      <c r="E9" s="160">
+        <v>-1.2973259780777705E-4</v>
+      </c>
+      <c r="F9" s="160">
+        <v>-6.1469074235460568E-3</v>
+      </c>
+      <c r="G9" s="160">
+        <v>2.2110525732097177E-2</v>
+      </c>
+      <c r="H9" s="160">
+        <v>2.5176490870686498E-2</v>
+      </c>
+      <c r="I9" s="160">
+        <v>2.7063015906224241E-2</v>
+      </c>
+      <c r="J9" s="160">
+        <v>5.2181504250876073E-2</v>
+      </c>
+      <c r="K9" s="160">
+        <v>-5.3059756291271032E-4</v>
+      </c>
+      <c r="L9" s="160">
+        <v>5.9412258874830121E-3</v>
+      </c>
+      <c r="M9" s="160">
+        <v>-6.7760729442727999E-3</v>
+      </c>
+      <c r="N9" s="160">
+        <v>9.0552831471905904E-6</v>
+      </c>
+      <c r="O9" s="160">
+        <v>-9.1704375216168948E-2</v>
+      </c>
+      <c r="P9" s="160">
+        <v>-2.3045338051309681E-3</v>
+      </c>
+      <c r="Q9" s="160">
+        <v>4.785944226724563E-3</v>
+      </c>
+      <c r="R9" s="160">
+        <v>-1.1164115771577143E-4</v>
+      </c>
+      <c r="S9" s="160">
+        <v>1.5601242939888739E-2</v>
+      </c>
+      <c r="T9" s="160">
+        <v>1.63234069968211E-2</v>
+      </c>
+      <c r="U9" s="160">
+        <v>-5.0697558200766435E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A10" s="161" t="s">
+        <v>70</v>
+      </c>
+      <c r="B10" s="161">
+        <v>-5.9759194525392391E-2</v>
+      </c>
+      <c r="C10" s="160">
+        <v>-1.337126851430994E-5</v>
+      </c>
+      <c r="D10" s="160">
+        <v>1.3334274550695201E-4</v>
+      </c>
+      <c r="E10" s="160">
+        <v>-2.0235229055515656E-6</v>
+      </c>
+      <c r="F10" s="160">
+        <v>6.9025246257722612E-4</v>
+      </c>
+      <c r="G10" s="160">
+        <v>-8.1411571659570792E-5</v>
+      </c>
+      <c r="H10" s="160">
+        <v>-7.311322364202729E-5</v>
+      </c>
+      <c r="I10" s="160">
+        <v>-2.015476968341757E-4</v>
+      </c>
+      <c r="J10" s="160">
+        <v>-5.3059756291271032E-4</v>
+      </c>
+      <c r="K10" s="160">
+        <v>4.7802212812020079E-4</v>
+      </c>
+      <c r="L10" s="160">
+        <v>-2.1131888499457906E-3</v>
+      </c>
+      <c r="M10" s="160">
+        <v>-2.4161411984220589E-3</v>
+      </c>
+      <c r="N10" s="160">
+        <v>-2.7976871750422451E-3</v>
+      </c>
+      <c r="O10" s="160">
+        <v>-9.439156383371318E-3</v>
+      </c>
+      <c r="P10" s="160">
+        <v>-8.2840543675118746E-5</v>
+      </c>
+      <c r="Q10" s="160">
+        <v>1.2550483094334419E-3</v>
+      </c>
+      <c r="R10" s="160">
+        <v>-2.6131583247368863E-5</v>
+      </c>
+      <c r="S10" s="160">
+        <v>7.5808524268866509E-5</v>
+      </c>
+      <c r="T10" s="160">
+        <v>5.9071232630555134E-4</v>
+      </c>
+      <c r="U10" s="160">
+        <v>-2.2741343752877619E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A11" s="161" t="s">
+        <v>71</v>
+      </c>
+      <c r="B11" s="161">
+        <v>-1.1613913824676128</v>
+      </c>
+      <c r="C11" s="160">
+        <v>-2.1891856823406438E-3</v>
+      </c>
+      <c r="D11" s="160">
+        <v>7.791539839853822E-4</v>
+      </c>
+      <c r="E11" s="160">
+        <v>-3.7146698134853394E-5</v>
+      </c>
+      <c r="F11" s="160">
+        <v>-4.7981931064700941E-3</v>
+      </c>
+      <c r="G11" s="160">
+        <v>-3.025506512017077E-3</v>
+      </c>
+      <c r="H11" s="160">
+        <v>1.3964214578385432E-3</v>
+      </c>
+      <c r="I11" s="160">
+        <v>-1.7655392515956124E-4</v>
+      </c>
+      <c r="J11" s="160">
+        <v>5.9412258874830121E-3</v>
+      </c>
+      <c r="K11" s="160">
+        <v>-2.1131888499457906E-3</v>
+      </c>
+      <c r="L11" s="160">
+        <v>0.10316938024489489</v>
+      </c>
+      <c r="M11" s="160">
+        <v>1.5066482152069063E-2</v>
+      </c>
+      <c r="N11" s="160">
+        <v>1.544205795626062E-2</v>
+      </c>
+      <c r="O11" s="160">
+        <v>2.8451199513488346E-2</v>
+      </c>
+      <c r="P11" s="160">
+        <v>-3.4478558931806758E-3</v>
+      </c>
+      <c r="Q11" s="160">
+        <v>-4.1197837299688581E-3</v>
+      </c>
+      <c r="R11" s="160">
+        <v>1.0180707743289059E-4</v>
+      </c>
+      <c r="S11" s="160">
+        <v>-6.094292962924382E-3</v>
+      </c>
+      <c r="T11" s="160">
+        <v>1.6897360108281117E-3</v>
+      </c>
+      <c r="U11" s="160">
+        <v>7.324165423245077E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A12" s="161" t="s">
+        <v>72</v>
+      </c>
+      <c r="B12" s="161">
+        <v>-0.22002905979608275</v>
+      </c>
+      <c r="C12" s="160">
+        <v>5.6669764918504048E-5</v>
+      </c>
+      <c r="D12" s="160">
+        <v>-9.0173638339487092E-3</v>
+      </c>
+      <c r="E12" s="160">
+        <v>1.8057494798948739E-4</v>
+      </c>
+      <c r="F12" s="160">
+        <v>3.0743777002507147E-3</v>
+      </c>
+      <c r="G12" s="160">
+        <v>-4.7033628432151843E-3</v>
+      </c>
+      <c r="H12" s="160">
+        <v>-6.4555702985388879E-3</v>
+      </c>
+      <c r="I12" s="160">
+        <v>-2.6172577357264108E-3</v>
+      </c>
+      <c r="J12" s="160">
+        <v>-6.7760729442727999E-3</v>
+      </c>
+      <c r="K12" s="160">
+        <v>-2.4161411984220589E-3</v>
+      </c>
+      <c r="L12" s="160">
+        <v>1.5066482152069063E-2</v>
+      </c>
+      <c r="M12" s="160">
+        <v>6.4892287160260298E-2</v>
+      </c>
+      <c r="N12" s="160">
+        <v>2.1136409211224998E-2</v>
+      </c>
+      <c r="O12" s="160">
+        <v>0.13908610264268956</v>
+      </c>
+      <c r="P12" s="160">
+        <v>4.3193058640607872E-3</v>
+      </c>
+      <c r="Q12" s="160">
+        <v>-9.6110776307609253E-3</v>
+      </c>
+      <c r="R12" s="160">
+        <v>2.2636258053497895E-4</v>
+      </c>
+      <c r="S12" s="160">
+        <v>-2.4827671609122595E-3</v>
+      </c>
+      <c r="T12" s="160">
+        <v>-1.0293215560079266E-2</v>
+      </c>
+      <c r="U12" s="160">
+        <v>0.13260379638600861</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A13" s="161" t="s">
+        <v>73</v>
+      </c>
+      <c r="B13" s="161">
+        <v>-0.12919115493816261</v>
+      </c>
+      <c r="C13" s="160">
+        <v>5.1510873478297331E-4</v>
+      </c>
+      <c r="D13" s="160">
+        <v>-2.0242235946012235E-2</v>
+      </c>
+      <c r="E13" s="160">
+        <v>4.6870459206550439E-4</v>
+      </c>
+      <c r="F13" s="160">
+        <v>1.016704010825858E-2</v>
+      </c>
+      <c r="G13" s="160">
+        <v>3.0933175404866051E-3</v>
+      </c>
+      <c r="H13" s="160">
+        <v>-4.5476122960031E-3</v>
+      </c>
+      <c r="I13" s="160">
+        <v>2.4354976656682545E-3</v>
+      </c>
+      <c r="J13" s="160">
+        <v>9.0552831471905904E-6</v>
+      </c>
+      <c r="K13" s="160">
+        <v>-2.7976871750422451E-3</v>
+      </c>
+      <c r="L13" s="160">
+        <v>1.544205795626062E-2</v>
+      </c>
+      <c r="M13" s="160">
+        <v>2.1136409211224998E-2</v>
+      </c>
+      <c r="N13" s="160">
+        <v>0.10294148874756442</v>
+      </c>
+      <c r="O13" s="160">
+        <v>0.24261511497454488</v>
+      </c>
+      <c r="P13" s="160">
+        <v>1.2051320436974702E-3</v>
+      </c>
+      <c r="Q13" s="160">
+        <v>-9.5460473362435197E-2</v>
+      </c>
+      <c r="R13" s="160">
+        <v>1.9473194726287004E-3</v>
+      </c>
+      <c r="S13" s="160">
+        <v>-1.0872883096165787E-2</v>
+      </c>
+      <c r="T13" s="160">
+        <v>-4.3427287006759198E-3</v>
+      </c>
+      <c r="U13" s="160">
+        <v>1.1932366704602</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A14" s="161" t="s">
+        <v>74</v>
+      </c>
+      <c r="B14" s="161">
+        <v>-31.824778747635925</v>
+      </c>
+      <c r="C14" s="160">
+        <v>8.7880342538172257E-2</v>
+      </c>
+      <c r="D14" s="160">
+        <v>-1.3986035022020817</v>
+      </c>
+      <c r="E14" s="160">
+        <v>2.9040910348742736E-2</v>
+      </c>
+      <c r="F14" s="160">
+        <v>2.9830211602031587E-2</v>
+      </c>
+      <c r="G14" s="160">
+        <v>-8.5386238867528275E-2</v>
+      </c>
+      <c r="H14" s="160">
+        <v>-5.9647244943152766E-2</v>
+      </c>
+      <c r="I14" s="160">
+        <v>-0.11441747715922801</v>
+      </c>
+      <c r="J14" s="160">
+        <v>-9.1704375216168948E-2</v>
+      </c>
+      <c r="K14" s="160">
+        <v>-9.439156383371318E-3</v>
+      </c>
+      <c r="L14" s="160">
+        <v>2.8451199513488346E-2</v>
+      </c>
+      <c r="M14" s="160">
+        <v>0.13908610264268956</v>
+      </c>
+      <c r="N14" s="160">
+        <v>0.24261511497454488</v>
+      </c>
+      <c r="O14" s="160">
+        <v>16.334908915481648</v>
+      </c>
+      <c r="P14" s="160">
+        <v>-1.9599056468963816E-2</v>
+      </c>
+      <c r="Q14" s="160">
+        <v>-1.0191472114811821</v>
+      </c>
+      <c r="R14" s="160">
+        <v>2.1160947486051039E-2</v>
+      </c>
+      <c r="S14" s="160">
+        <v>-7.495332768834248E-2</v>
+      </c>
+      <c r="T14" s="160">
+        <v>-5.9532220142608311E-2</v>
+      </c>
+      <c r="U14" s="160">
+        <v>12.36857040298562</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A15" s="161" t="s">
+        <v>75</v>
+      </c>
+      <c r="B15" s="161">
+        <v>-0.86026861165285218</v>
+      </c>
+      <c r="C15" s="160">
+        <v>1.439055119746919E-3</v>
+      </c>
+      <c r="D15" s="160">
+        <v>1.8470049044626933E-3</v>
+      </c>
+      <c r="E15" s="160">
+        <v>-4.7722422693127043E-5</v>
+      </c>
+      <c r="F15" s="160">
+        <v>4.8554709112269435E-3</v>
+      </c>
+      <c r="G15" s="160">
+        <v>-2.8873970464742861E-3</v>
+      </c>
+      <c r="H15" s="160">
+        <v>-5.5379760447134187E-3</v>
+      </c>
+      <c r="I15" s="160">
+        <v>-2.407540674298457E-3</v>
+      </c>
+      <c r="J15" s="160">
+        <v>-2.3045338051309681E-3</v>
+      </c>
+      <c r="K15" s="160">
+        <v>-8.2840543675118746E-5</v>
+      </c>
+      <c r="L15" s="160">
+        <v>-3.4478558931806758E-3</v>
+      </c>
+      <c r="M15" s="160">
+        <v>4.3193058640607872E-3</v>
+      </c>
+      <c r="N15" s="160">
+        <v>1.2051320436974702E-3</v>
+      </c>
+      <c r="O15" s="160">
+        <v>-1.9599056468963816E-2</v>
+      </c>
+      <c r="P15" s="160">
+        <v>4.1432651153713244E-2</v>
+      </c>
+      <c r="Q15" s="160">
+        <v>2.3177889100075698E-2</v>
+      </c>
+      <c r="R15" s="160">
+        <v>-4.79047280630629E-4</v>
+      </c>
+      <c r="S15" s="160">
+        <v>2.1898199223887938E-3</v>
+      </c>
+      <c r="T15" s="160">
+        <v>-4.1844998178358428E-3</v>
+      </c>
+      <c r="U15" s="160">
+        <v>-0.2974141363248014</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A16" s="161" t="s">
+        <v>76</v>
+      </c>
+      <c r="B16" s="161">
+        <v>6.2263464240763486</v>
+      </c>
+      <c r="C16" s="160">
+        <v>-4.0689315322597159E-4</v>
+      </c>
+      <c r="D16" s="160">
+        <v>0.10415682330628889</v>
+      </c>
+      <c r="E16" s="160">
+        <v>-2.5784274725718743E-3</v>
+      </c>
+      <c r="F16" s="160">
+        <v>-4.9467139915576913E-2</v>
+      </c>
+      <c r="G16" s="160">
+        <v>-2.3387825911462767E-2</v>
+      </c>
+      <c r="H16" s="160">
+        <v>2.6798582470341507E-2</v>
+      </c>
+      <c r="I16" s="160">
+        <v>3.5110494572182099E-3</v>
+      </c>
+      <c r="J16" s="160">
+        <v>4.785944226724563E-3</v>
+      </c>
+      <c r="K16" s="160">
+        <v>1.2550483094334419E-3</v>
+      </c>
+      <c r="L16" s="160">
+        <v>-4.1197837299688581E-3</v>
+      </c>
+      <c r="M16" s="160">
+        <v>-9.6110776307609253E-3</v>
+      </c>
+      <c r="N16" s="160">
+        <v>-9.5460473362435197E-2</v>
+      </c>
+      <c r="O16" s="160">
+        <v>-1.0191472114811821</v>
+      </c>
+      <c r="P16" s="160">
+        <v>2.3177889100075698E-2</v>
+      </c>
+      <c r="Q16" s="160">
+        <v>0.79912571660915388</v>
+      </c>
+      <c r="R16" s="160">
+        <v>-1.6280227139184957E-2</v>
+      </c>
+      <c r="S16" s="160">
+        <v>3.4794836640971327E-2</v>
+      </c>
+      <c r="T16" s="160">
+        <v>9.5379348219153393E-3</v>
+      </c>
+      <c r="U16" s="160">
+        <v>-9.7334215216833275</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A17" s="161" t="s">
+        <v>77</v>
+      </c>
+      <c r="B17" s="161">
+        <v>-0.10696576698473485</v>
+      </c>
+      <c r="C17" s="160">
+        <v>1.110339955305822E-5</v>
+      </c>
+      <c r="D17" s="160">
+        <v>-2.1698494664189475E-3</v>
+      </c>
+      <c r="E17" s="160">
+        <v>5.3843878149397985E-5</v>
+      </c>
+      <c r="F17" s="160">
+        <v>1.0553442399555634E-3</v>
+      </c>
+      <c r="G17" s="160">
+        <v>4.7286609447689046E-4</v>
+      </c>
+      <c r="H17" s="160">
+        <v>-5.7113880525171763E-4</v>
+      </c>
+      <c r="I17" s="160">
+        <v>-7.5253787542500675E-5</v>
+      </c>
+      <c r="J17" s="160">
+        <v>-1.1164115771577143E-4</v>
+      </c>
+      <c r="K17" s="160">
+        <v>-2.6131583247368863E-5</v>
+      </c>
+      <c r="L17" s="160">
+        <v>1.0180707743289059E-4</v>
+      </c>
+      <c r="M17" s="160">
+        <v>2.2636258053497895E-4</v>
+      </c>
+      <c r="N17" s="160">
+        <v>1.9473194726287004E-3</v>
+      </c>
+      <c r="O17" s="160">
+        <v>2.1160947486051039E-2</v>
+      </c>
+      <c r="P17" s="160">
+        <v>-4.79047280630629E-4</v>
+      </c>
+      <c r="Q17" s="160">
+        <v>-1.6280227139184957E-2</v>
+      </c>
+      <c r="R17" s="160">
+        <v>3.3290352391684129E-4</v>
+      </c>
+      <c r="S17" s="160">
+        <v>-6.7396966928173936E-4</v>
+      </c>
+      <c r="T17" s="160">
+        <v>-2.2026674263010085E-4</v>
+      </c>
+      <c r="U17" s="160">
+        <v>0.19759101965327769</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A18" s="161" t="s">
+        <v>78</v>
+      </c>
+      <c r="B18" s="161">
+        <v>-0.49295338017573992</v>
+      </c>
+      <c r="C18" s="160">
+        <v>-1.4701051190887156E-3</v>
+      </c>
+      <c r="D18" s="160">
+        <v>6.5100352188719188E-3</v>
+      </c>
+      <c r="E18" s="160">
+        <v>-1.5651390419824432E-4</v>
+      </c>
+      <c r="F18" s="160">
+        <v>-7.2055629481296447E-3</v>
+      </c>
+      <c r="G18" s="160">
+        <v>2.3369530589833973E-2</v>
+      </c>
+      <c r="H18" s="160">
+        <v>2.1644665590256369E-2</v>
+      </c>
+      <c r="I18" s="160">
+        <v>1.6366262480138026E-2</v>
+      </c>
+      <c r="J18" s="160">
+        <v>1.5601242939888739E-2</v>
+      </c>
+      <c r="K18" s="160">
+        <v>7.5808524268866509E-5</v>
+      </c>
+      <c r="L18" s="160">
+        <v>-6.094292962924382E-3</v>
+      </c>
+      <c r="M18" s="160">
+        <v>-2.4827671609122595E-3</v>
+      </c>
+      <c r="N18" s="160">
+        <v>-1.0872883096165787E-2</v>
+      </c>
+      <c r="O18" s="160">
+        <v>-7.495332768834248E-2</v>
+      </c>
+      <c r="P18" s="160">
+        <v>2.1898199223887938E-3</v>
+      </c>
+      <c r="Q18" s="160">
+        <v>3.4794836640971327E-2</v>
+      </c>
+      <c r="R18" s="160">
+        <v>-6.7396966928173936E-4</v>
+      </c>
+      <c r="S18" s="160">
+        <v>0.11909614688779115</v>
+      </c>
+      <c r="T18" s="160">
+        <v>3.7920589894415949E-2</v>
+      </c>
+      <c r="U18" s="160">
+        <v>-0.47856495314507796</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A19" s="161" t="s">
+        <v>79</v>
+      </c>
+      <c r="B19" s="161">
+        <v>-0.34501585542851426</v>
+      </c>
+      <c r="C19" s="160">
+        <v>-9.1701749141058345E-4</v>
+      </c>
+      <c r="D19" s="160">
+        <v>4.4845659265097667E-3</v>
+      </c>
+      <c r="E19" s="160">
+        <v>-1.2029668913989115E-4</v>
+      </c>
+      <c r="F19" s="160">
+        <v>-6.0152523808594633E-3</v>
+      </c>
+      <c r="G19" s="160">
+        <v>2.4267537119822602E-2</v>
+      </c>
+      <c r="H19" s="160">
+        <v>2.2575139577819744E-2</v>
+      </c>
+      <c r="I19" s="160">
+        <v>1.5769792226923096E-2</v>
+      </c>
+      <c r="J19" s="160">
+        <v>1.63234069968211E-2</v>
+      </c>
+      <c r="K19" s="160">
+        <v>5.9071232630555134E-4</v>
+      </c>
+      <c r="L19" s="160">
+        <v>1.6897360108281117E-3</v>
+      </c>
+      <c r="M19" s="160">
+        <v>-1.0293215560079266E-2</v>
+      </c>
+      <c r="N19" s="160">
+        <v>-4.3427287006759198E-3</v>
+      </c>
+      <c r="O19" s="160">
+        <v>-5.9532220142608311E-2</v>
+      </c>
+      <c r="P19" s="160">
+        <v>-4.1844998178358428E-3</v>
+      </c>
+      <c r="Q19" s="160">
+        <v>9.5379348219153393E-3</v>
+      </c>
+      <c r="R19" s="160">
+        <v>-2.2026674263010085E-4</v>
+      </c>
+      <c r="S19" s="160">
+        <v>3.7920589894415949E-2</v>
+      </c>
+      <c r="T19" s="160">
+        <v>6.1113114118783278E-2</v>
+      </c>
+      <c r="U19" s="160">
+        <v>-0.14165162191459829</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A20" s="161" t="s">
+        <v>80</v>
+      </c>
+      <c r="B20" s="161">
+        <v>-86.584533835960286</v>
+      </c>
+      <c r="C20" s="160">
+        <v>1.8946138227211688E-3</v>
+      </c>
+      <c r="D20" s="160">
+        <v>-1.2407128942348631</v>
+      </c>
+      <c r="E20" s="160">
+        <v>3.0597157804174015E-2</v>
+      </c>
+      <c r="F20" s="160">
+        <v>0.52650696178581669</v>
+      </c>
+      <c r="G20" s="160">
+        <v>0.26789795838039099</v>
+      </c>
+      <c r="H20" s="160">
+        <v>-0.32507577205139465</v>
+      </c>
+      <c r="I20" s="160">
+        <v>-5.0233387354936598E-2</v>
+      </c>
+      <c r="J20" s="160">
+        <v>-5.0697558200766435E-2</v>
+      </c>
+      <c r="K20" s="160">
+        <v>-2.2741343752877619E-2</v>
+      </c>
+      <c r="L20" s="160">
+        <v>7.324165423245077E-2</v>
+      </c>
+      <c r="M20" s="160">
+        <v>0.13260379638600861</v>
+      </c>
+      <c r="N20" s="160">
+        <v>1.1932366704602</v>
+      </c>
+      <c r="O20" s="160">
+        <v>12.36857040298562</v>
+      </c>
+      <c r="P20" s="160">
+        <v>-0.2974141363248014</v>
+      </c>
+      <c r="Q20" s="160">
+        <v>-9.7334215216833275</v>
+      </c>
+      <c r="R20" s="160">
+        <v>0.19759101965327769</v>
+      </c>
+      <c r="S20" s="160">
+        <v>-0.47856495314507796</v>
+      </c>
+      <c r="T20" s="160">
+        <v>-0.14165162191459829</v>
+      </c>
+      <c r="U20" s="160">
+        <v>119.15331153695513</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added .do files that ensure process-specific time trends
</commit_message>
<xml_diff>
--- a/input/PL/reg_education.xlsx
+++ b/input/PL/reg_education.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pineapple/IdeaProjects/SimPathsEU_JAN/input/PL/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95C8DB19-A71A-CF47-9FE5-5E3F66E94967}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88FC8921-E772-AB43-ACFD-861CC398D0C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13460" yWindow="2520" windowWidth="30240" windowHeight="18880" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13460" yWindow="2520" windowWidth="30240" windowHeight="18880" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="87">
   <si>
     <t>Description:</t>
   </si>
@@ -249,12 +249,6 @@
     <t>PL10_</t>
   </si>
   <si>
-    <t>Year_transformed_</t>
-  </si>
-  <si>
-    <t>Year_transformed_sq_</t>
-  </si>
-  <si>
     <t>Y2022_</t>
   </si>
   <si>
@@ -277,13 +271,28 @@
   </si>
   <si>
     <t>E2a - Educational attainment</t>
+  </si>
+  <si>
+    <t>Year_transformed_E2a_</t>
+  </si>
+  <si>
+    <t>Year_transformed_sq_E2a_</t>
+  </si>
+  <si>
+    <t>Year_transformed_E1b</t>
+  </si>
+  <si>
+    <t>Year_transformed_sq_E1b</t>
+  </si>
+  <si>
+    <t>Year_transformed_E1a</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="144" x14ac:knownFonts="1">
+  <fonts count="142" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -338,16 +347,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -2035,7 +2034,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="144">
+  <cellXfs count="145">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -2161,25 +2160,26 @@
     <xf numFmtId="2" fontId="122" fillId="0" borderId="122" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="123" fillId="0" borderId="123" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="124" fillId="0" borderId="124" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="125" fillId="0" borderId="125" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="126" fillId="0" borderId="126" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="127" fillId="0" borderId="127" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="128" fillId="0" borderId="128" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="129" fillId="0" borderId="129" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="130" fillId="0" borderId="130" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="131" fillId="0" borderId="131" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="132" fillId="0" borderId="132" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="133" fillId="0" borderId="133" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="134" fillId="0" borderId="134" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="135" fillId="0" borderId="135" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="136" fillId="0" borderId="136" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="137" fillId="0" borderId="137" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="138" fillId="0" borderId="138" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="139" fillId="0" borderId="139" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="140" fillId="0" borderId="140" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="141" fillId="0" borderId="141" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="142" fillId="0" borderId="142" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="143" fillId="0" borderId="143" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="125" fillId="0" borderId="126" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="126" fillId="0" borderId="128" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="127" fillId="0" borderId="129" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="128" fillId="0" borderId="130" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="129" fillId="0" borderId="131" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="130" fillId="0" borderId="132" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="131" fillId="0" borderId="133" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="132" fillId="0" borderId="134" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="133" fillId="0" borderId="135" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="134" fillId="0" borderId="136" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="135" fillId="0" borderId="137" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="136" fillId="0" borderId="138" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="137" fillId="0" borderId="139" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="138" fillId="0" borderId="140" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="139" fillId="0" borderId="141" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="140" fillId="0" borderId="142" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="141" fillId="0" borderId="143" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="10" fillId="0" borderId="125" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="10" fillId="0" borderId="127" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2677,8 +2677,8 @@
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" s="143" t="s">
-        <v>83</v>
+      <c r="A13" s="141" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
@@ -2706,8 +2706,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:U20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="V2" sqref="V2:V20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q2" sqref="Q2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2764,8 +2764,8 @@
       <c r="P1" t="s">
         <v>33</v>
       </c>
-      <c r="Q1" t="s">
-        <v>34</v>
+      <c r="Q1" s="144" t="s">
+        <v>86</v>
       </c>
       <c r="R1" t="s">
         <v>35</v>
@@ -3691,8 +3691,8 @@
       </c>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>34</v>
+      <c r="A16" s="144" t="s">
+        <v>86</v>
       </c>
       <c r="B16">
         <v>-4.9701210281089779E-2</v>
@@ -4025,7 +4025,7 @@
   <dimension ref="A1:S18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="Q1" sqref="Q1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4079,11 +4079,11 @@
       <c r="O1" t="s">
         <v>33</v>
       </c>
-      <c r="P1" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>51</v>
+      <c r="P1" s="144" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q1" s="144" t="s">
+        <v>85</v>
       </c>
       <c r="R1" t="s">
         <v>35</v>
@@ -4860,8 +4860,8 @@
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>34</v>
+      <c r="A15" s="144" t="s">
+        <v>84</v>
       </c>
       <c r="B15">
         <v>-0.31553104949630212</v>
@@ -4919,8 +4919,8 @@
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>51</v>
+      <c r="A16" s="144" t="s">
+        <v>85</v>
       </c>
       <c r="B16">
         <v>1.0582240239214599E-2</v>
@@ -5480,8 +5480,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:R17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S2" sqref="S2:S17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5517,32 +5517,32 @@
       <c r="I1" t="s">
         <v>73</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="144" t="s">
+        <v>82</v>
+      </c>
+      <c r="K1" s="144" t="s">
+        <v>83</v>
+      </c>
+      <c r="L1" t="s">
         <v>74</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>75</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>76</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
         <v>77</v>
       </c>
-      <c r="N1" t="s">
+      <c r="P1" t="s">
         <v>78</v>
       </c>
-      <c r="O1" t="s">
+      <c r="Q1" t="s">
         <v>79</v>
       </c>
-      <c r="P1" t="s">
+      <c r="R1" t="s">
         <v>80</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>81</v>
-      </c>
-      <c r="R1" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.2">
@@ -5938,10 +5938,10 @@
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A9" s="125" t="s">
-        <v>74</v>
-      </c>
-      <c r="B9" s="126">
+      <c r="A9" s="142" t="s">
+        <v>82</v>
+      </c>
+      <c r="B9" s="125">
         <v>0.18640381066811282</v>
       </c>
       <c r="C9">
@@ -5994,10 +5994,10 @@
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A10" s="127" t="s">
-        <v>75</v>
-      </c>
-      <c r="B10" s="128">
+      <c r="A10" s="143" t="s">
+        <v>83</v>
+      </c>
+      <c r="B10" s="126">
         <v>-6.6075553534049748E-3</v>
       </c>
       <c r="C10">
@@ -6050,10 +6050,10 @@
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A11" s="129" t="s">
-        <v>76</v>
-      </c>
-      <c r="B11" s="130">
+      <c r="A11" s="127" t="s">
+        <v>74</v>
+      </c>
+      <c r="B11" s="128">
         <v>-0.61312845869547283</v>
       </c>
       <c r="C11">
@@ -6106,10 +6106,10 @@
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A12" s="131" t="s">
-        <v>77</v>
-      </c>
-      <c r="B12" s="132">
+      <c r="A12" s="129" t="s">
+        <v>75</v>
+      </c>
+      <c r="B12" s="130">
         <v>-7.819005525547813</v>
       </c>
       <c r="C12">
@@ -6162,10 +6162,10 @@
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A13" s="133" t="s">
-        <v>78</v>
-      </c>
-      <c r="B13" s="134">
+      <c r="A13" s="131" t="s">
+        <v>76</v>
+      </c>
+      <c r="B13" s="132">
         <v>-0.57366523018618643</v>
       </c>
       <c r="C13">
@@ -6218,10 +6218,10 @@
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A14" s="135" t="s">
-        <v>79</v>
-      </c>
-      <c r="B14" s="136">
+      <c r="A14" s="133" t="s">
+        <v>77</v>
+      </c>
+      <c r="B14" s="134">
         <v>-1.726532244359815</v>
       </c>
       <c r="C14">
@@ -6274,10 +6274,10 @@
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A15" s="137" t="s">
-        <v>80</v>
-      </c>
-      <c r="B15" s="138">
+      <c r="A15" s="135" t="s">
+        <v>78</v>
+      </c>
+      <c r="B15" s="136">
         <v>5.0042998474953589E-2</v>
       </c>
       <c r="C15">
@@ -6330,10 +6330,10 @@
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A16" s="139" t="s">
-        <v>81</v>
-      </c>
-      <c r="B16" s="140">
+      <c r="A16" s="137" t="s">
+        <v>79</v>
+      </c>
+      <c r="B16" s="138">
         <v>0.22337779378170336</v>
       </c>
       <c r="C16">
@@ -6386,10 +6386,10 @@
       </c>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A17" s="141" t="s">
-        <v>82</v>
-      </c>
-      <c r="B17" s="142">
+      <c r="A17" s="139" t="s">
+        <v>80</v>
+      </c>
+      <c r="B17" s="140">
         <v>11.570207623900812</v>
       </c>
       <c r="C17">

</xml_diff>